<commit_message>
update runtime on browser
</commit_message>
<xml_diff>
--- a/evaluate/eval_result.xlsx
+++ b/evaluate/eval_result.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\beshar\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9986D6A2-8206-4945-99B0-4966D03BAF1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F2060B4-137C-444C-A9D3-21E315AAC314}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-93" yWindow="-93" windowWidth="20666" windowHeight="12266" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-93" yWindow="-93" windowWidth="20666" windowHeight="12266" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="AMTresult" sheetId="2" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="151">
   <si>
     <t>focal loss</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -639,6 +639,22 @@
   </si>
   <si>
     <t>AVG</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>on broswer</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>intel Ultra 7 255H</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>only inference (ms):</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>post-process time (ms):</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -876,7 +892,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1007,84 +1023,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1096,27 +1034,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1136,16 +1053,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1156,6 +1070,87 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1501,8 +1496,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:BL93"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B78" sqref="B78:C79"/>
+    <sheetView tabSelected="1" topLeftCell="A53" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q69" sqref="Q69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
@@ -1554,85 +1549,85 @@
       <c r="G1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H1" s="56" t="s">
+      <c r="H1" s="72" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="44"/>
-      <c r="P1" s="44"/>
-      <c r="Q1" s="57"/>
-      <c r="R1" s="56" t="s">
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="64"/>
+      <c r="P1" s="64"/>
+      <c r="Q1" s="73"/>
+      <c r="R1" s="72" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="57"/>
-      <c r="AB1" s="56" t="s">
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="73"/>
+      <c r="AB1" s="72" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="44"/>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="57"/>
-      <c r="AL1" s="56" t="s">
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="64"/>
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="64"/>
+      <c r="AH1" s="64"/>
+      <c r="AI1" s="64"/>
+      <c r="AJ1" s="64"/>
+      <c r="AK1" s="73"/>
+      <c r="AL1" s="72" t="s">
         <v>29</v>
       </c>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="44"/>
-      <c r="AR1" s="44"/>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="57"/>
-      <c r="AV1" s="56" t="s">
+      <c r="AM1" s="64"/>
+      <c r="AN1" s="64"/>
+      <c r="AO1" s="64"/>
+      <c r="AP1" s="64"/>
+      <c r="AQ1" s="64"/>
+      <c r="AR1" s="64"/>
+      <c r="AS1" s="64"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="73"/>
+      <c r="AV1" s="72" t="s">
         <v>30</v>
       </c>
-      <c r="AW1" s="44"/>
-      <c r="AX1" s="44"/>
-      <c r="AY1" s="44"/>
-      <c r="AZ1" s="44"/>
-      <c r="BA1" s="44"/>
-      <c r="BB1" s="44"/>
-      <c r="BC1" s="44"/>
-      <c r="BD1" s="44"/>
-      <c r="BE1" s="57"/>
-      <c r="BF1" s="45" t="s">
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="64"/>
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="73"/>
+      <c r="BF1" s="67" t="s">
         <v>53</v>
       </c>
-      <c r="BG1" s="44" t="s">
+      <c r="BG1" s="64" t="s">
         <v>7</v>
       </c>
-      <c r="BH1" s="44" t="s">
+      <c r="BH1" s="64" t="s">
         <v>8</v>
       </c>
-      <c r="BI1" s="45" t="s">
+      <c r="BI1" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="BJ1" s="45" t="s">
+      <c r="BJ1" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="BK1" s="45" t="s">
+      <c r="BK1" s="67" t="s">
         <v>11</v>
       </c>
-      <c r="BL1" s="45" t="s">
+      <c r="BL1" s="67" t="s">
         <v>12</v>
       </c>
     </row>
@@ -1640,79 +1635,79 @@
       <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="56" t="s">
+      <c r="H2" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="I2" s="44"/>
-      <c r="J2" s="44"/>
-      <c r="K2" s="44"/>
-      <c r="L2" s="44"/>
-      <c r="N2" s="44" t="s">
+      <c r="I2" s="64"/>
+      <c r="J2" s="64"/>
+      <c r="K2" s="64"/>
+      <c r="L2" s="64"/>
+      <c r="N2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="O2" s="44"/>
-      <c r="P2" s="44"/>
-      <c r="Q2" s="57"/>
-      <c r="R2" s="56" t="s">
+      <c r="O2" s="64"/>
+      <c r="P2" s="64"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="44"/>
-      <c r="T2" s="44"/>
-      <c r="U2" s="44"/>
-      <c r="V2" s="44"/>
+      <c r="S2" s="64"/>
+      <c r="T2" s="64"/>
+      <c r="U2" s="64"/>
+      <c r="V2" s="64"/>
       <c r="W2" s="5"/>
-      <c r="X2" s="44" t="s">
+      <c r="X2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="44"/>
-      <c r="Z2" s="44"/>
-      <c r="AA2" s="57"/>
-      <c r="AB2" s="56" t="s">
+      <c r="Y2" s="64"/>
+      <c r="Z2" s="64"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="AC2" s="44"/>
-      <c r="AD2" s="44"/>
-      <c r="AE2" s="44"/>
-      <c r="AF2" s="44"/>
-      <c r="AH2" s="44" t="s">
+      <c r="AC2" s="64"/>
+      <c r="AD2" s="64"/>
+      <c r="AE2" s="64"/>
+      <c r="AF2" s="64"/>
+      <c r="AH2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="AI2" s="44"/>
-      <c r="AJ2" s="44"/>
-      <c r="AK2" s="57"/>
-      <c r="AL2" s="56" t="s">
+      <c r="AI2" s="64"/>
+      <c r="AJ2" s="64"/>
+      <c r="AK2" s="73"/>
+      <c r="AL2" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="AM2" s="44"/>
-      <c r="AN2" s="44"/>
-      <c r="AO2" s="44"/>
-      <c r="AP2" s="44"/>
-      <c r="AR2" s="44" t="s">
+      <c r="AM2" s="64"/>
+      <c r="AN2" s="64"/>
+      <c r="AO2" s="64"/>
+      <c r="AP2" s="64"/>
+      <c r="AR2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="AS2" s="44"/>
-      <c r="AT2" s="44"/>
-      <c r="AU2" s="57"/>
-      <c r="AV2" s="56" t="s">
+      <c r="AS2" s="64"/>
+      <c r="AT2" s="64"/>
+      <c r="AU2" s="73"/>
+      <c r="AV2" s="72" t="s">
         <v>31</v>
       </c>
-      <c r="AW2" s="44"/>
-      <c r="AX2" s="44"/>
-      <c r="AY2" s="44"/>
-      <c r="AZ2" s="44"/>
-      <c r="BB2" s="44" t="s">
+      <c r="AW2" s="64"/>
+      <c r="AX2" s="64"/>
+      <c r="AY2" s="64"/>
+      <c r="AZ2" s="64"/>
+      <c r="BB2" s="64" t="s">
         <v>32</v>
       </c>
-      <c r="BC2" s="44"/>
-      <c r="BD2" s="44"/>
-      <c r="BE2" s="57"/>
-      <c r="BF2" s="44"/>
-      <c r="BG2" s="44"/>
-      <c r="BH2" s="44"/>
-      <c r="BI2" s="44"/>
-      <c r="BJ2" s="44"/>
-      <c r="BK2" s="44"/>
-      <c r="BL2" s="44"/>
+      <c r="BC2" s="64"/>
+      <c r="BD2" s="64"/>
+      <c r="BE2" s="73"/>
+      <c r="BF2" s="64"/>
+      <c r="BG2" s="64"/>
+      <c r="BH2" s="64"/>
+      <c r="BI2" s="64"/>
+      <c r="BJ2" s="64"/>
+      <c r="BK2" s="64"/>
+      <c r="BL2" s="64"/>
     </row>
     <row r="3" spans="1:64" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -1886,34 +1881,34 @@
       <c r="BE3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="BF3" s="44"/>
-      <c r="BG3" s="44"/>
-      <c r="BH3" s="44"/>
-      <c r="BI3" s="44"/>
-      <c r="BJ3" s="44"/>
-      <c r="BK3" s="44"/>
-      <c r="BL3" s="44"/>
+      <c r="BF3" s="64"/>
+      <c r="BG3" s="64"/>
+      <c r="BH3" s="64"/>
+      <c r="BI3" s="64"/>
+      <c r="BJ3" s="64"/>
+      <c r="BK3" s="64"/>
+      <c r="BL3" s="64"/>
     </row>
     <row r="4" spans="1:64" s="16" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="46" t="s">
+      <c r="A4" s="60" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C4" s="49" t="s">
+      <c r="C4" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D4" s="49" t="s">
+      <c r="D4" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="51" t="s">
+      <c r="E4" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="49" t="s">
+      <c r="F4" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="62" t="s">
+      <c r="G4" s="69" t="s">
         <v>56</v>
       </c>
       <c r="H4" s="17">
@@ -2071,13 +2066,13 @@
       </c>
     </row>
     <row r="5" spans="1:64" x14ac:dyDescent="0.45">
-      <c r="A5" s="47"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="45"/>
-      <c r="D5" s="45"/>
-      <c r="E5" s="44"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="63"/>
+      <c r="A5" s="61"/>
+      <c r="B5" s="64"/>
+      <c r="C5" s="67"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="67"/>
+      <c r="G5" s="70"/>
       <c r="H5" s="2">
         <v>0.20873</v>
       </c>
@@ -2230,13 +2225,13 @@
       </c>
     </row>
     <row r="6" spans="1:64" x14ac:dyDescent="0.45">
-      <c r="A6" s="47"/>
-      <c r="B6" s="44"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="44"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="63"/>
+      <c r="A6" s="61"/>
+      <c r="B6" s="64"/>
+      <c r="C6" s="67"/>
+      <c r="D6" s="67"/>
+      <c r="E6" s="64"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="70"/>
       <c r="H6" s="2">
         <v>0.16517999999999999</v>
       </c>
@@ -2389,13 +2384,13 @@
       </c>
     </row>
     <row r="7" spans="1:64" x14ac:dyDescent="0.45">
-      <c r="A7" s="47"/>
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="44"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="63"/>
+      <c r="A7" s="61"/>
+      <c r="B7" s="64"/>
+      <c r="C7" s="67"/>
+      <c r="D7" s="67"/>
+      <c r="E7" s="64"/>
+      <c r="F7" s="67"/>
+      <c r="G7" s="70"/>
       <c r="H7" s="2">
         <v>0.22</v>
       </c>
@@ -2548,13 +2543,13 @@
       </c>
     </row>
     <row r="8" spans="1:64" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="48"/>
-      <c r="B8" s="50"/>
-      <c r="C8" s="58"/>
-      <c r="D8" s="58"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="64"/>
+      <c r="A8" s="62"/>
+      <c r="B8" s="65"/>
+      <c r="C8" s="68"/>
+      <c r="D8" s="68"/>
+      <c r="E8" s="65"/>
+      <c r="F8" s="68"/>
+      <c r="G8" s="71"/>
       <c r="H8" s="26">
         <v>0.18129000000000001</v>
       </c>
@@ -3023,25 +3018,25 @@
       </c>
     </row>
     <row r="11" spans="1:64" x14ac:dyDescent="0.45">
-      <c r="A11" s="44" t="s">
+      <c r="A11" s="64" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="44" t="s">
+      <c r="B11" s="64" t="s">
         <v>65</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="C11" s="67" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="D11" s="67" t="s">
         <v>23</v>
       </c>
-      <c r="E11" s="44" t="s">
+      <c r="E11" s="64" t="s">
         <v>19</v>
       </c>
-      <c r="F11" s="65" t="s">
+      <c r="F11" s="74" t="s">
         <v>24</v>
       </c>
-      <c r="G11" s="45" t="s">
+      <c r="G11" s="67" t="s">
         <v>55</v>
       </c>
       <c r="H11" s="2">
@@ -3196,13 +3191,13 @@
       </c>
     </row>
     <row r="12" spans="1:64" x14ac:dyDescent="0.45">
-      <c r="A12" s="44"/>
-      <c r="B12" s="44"/>
-      <c r="C12" s="44"/>
-      <c r="D12" s="44"/>
-      <c r="E12" s="44"/>
-      <c r="F12" s="53"/>
-      <c r="G12" s="44"/>
+      <c r="A12" s="64"/>
+      <c r="B12" s="64"/>
+      <c r="C12" s="64"/>
+      <c r="D12" s="64"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="75"/>
+      <c r="G12" s="64"/>
       <c r="H12" s="2">
         <v>0.15487999999999999</v>
       </c>
@@ -3355,13 +3350,13 @@
       </c>
     </row>
     <row r="13" spans="1:64" x14ac:dyDescent="0.45">
-      <c r="A13" s="44"/>
-      <c r="B13" s="44"/>
-      <c r="C13" s="44"/>
-      <c r="D13" s="44"/>
-      <c r="E13" s="44"/>
-      <c r="F13" s="53"/>
-      <c r="G13" s="44"/>
+      <c r="A13" s="64"/>
+      <c r="B13" s="64"/>
+      <c r="C13" s="64"/>
+      <c r="D13" s="64"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="75"/>
+      <c r="G13" s="64"/>
       <c r="H13" s="2">
         <v>0.15487999999999999</v>
       </c>
@@ -3514,25 +3509,25 @@
       </c>
     </row>
     <row r="14" spans="1:64" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="61" t="s">
+      <c r="A14" s="76" t="s">
         <v>89</v>
       </c>
-      <c r="B14" s="51" t="s">
+      <c r="B14" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="49" t="s">
+      <c r="C14" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="49" t="s">
+      <c r="D14" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="E14" s="51" t="s">
+      <c r="E14" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F14" s="52" t="s">
+      <c r="F14" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G14" s="49" t="s">
+      <c r="G14" s="66" t="s">
         <v>55</v>
       </c>
       <c r="H14" s="17">
@@ -3687,13 +3682,13 @@
       </c>
     </row>
     <row r="15" spans="1:64" x14ac:dyDescent="0.45">
-      <c r="A15" s="59"/>
-      <c r="B15" s="44"/>
-      <c r="C15" s="44"/>
-      <c r="D15" s="44"/>
-      <c r="E15" s="44"/>
-      <c r="F15" s="53"/>
-      <c r="G15" s="44"/>
+      <c r="A15" s="77"/>
+      <c r="B15" s="64"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="75"/>
+      <c r="G15" s="64"/>
       <c r="H15" s="2">
         <v>0.18</v>
       </c>
@@ -3846,13 +3841,13 @@
       </c>
     </row>
     <row r="16" spans="1:64" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="60"/>
-      <c r="B16" s="50"/>
-      <c r="C16" s="50"/>
-      <c r="D16" s="50"/>
-      <c r="E16" s="50"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="50"/>
+      <c r="A16" s="78"/>
+      <c r="B16" s="65"/>
+      <c r="C16" s="65"/>
+      <c r="D16" s="65"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="80"/>
+      <c r="G16" s="65"/>
       <c r="H16" s="26">
         <v>0.14893000000000001</v>
       </c>
@@ -4005,25 +4000,25 @@
       </c>
     </row>
     <row r="17" spans="1:57" s="16" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="51" t="s">
+      <c r="A17" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="B17" s="51" t="s">
+      <c r="B17" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="49" t="s">
+      <c r="C17" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D17" s="49" t="s">
+      <c r="D17" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="E17" s="51" t="s">
+      <c r="E17" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F17" s="55" t="s">
+      <c r="F17" s="79" t="s">
         <v>90</v>
       </c>
-      <c r="G17" s="51" t="s">
+      <c r="G17" s="63" t="s">
         <v>56</v>
       </c>
       <c r="H17" s="17">
@@ -4178,13 +4173,13 @@
       </c>
     </row>
     <row r="18" spans="1:57" x14ac:dyDescent="0.45">
-      <c r="A18" s="44"/>
-      <c r="B18" s="44"/>
-      <c r="C18" s="45"/>
-      <c r="D18" s="45"/>
-      <c r="E18" s="44"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="44"/>
+      <c r="A18" s="64"/>
+      <c r="B18" s="64"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="64"/>
+      <c r="F18" s="75"/>
+      <c r="G18" s="64"/>
       <c r="H18" s="2">
         <v>0.12056</v>
       </c>
@@ -4337,13 +4332,13 @@
       </c>
     </row>
     <row r="19" spans="1:57" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="50"/>
-      <c r="B19" s="50"/>
-      <c r="C19" s="58"/>
-      <c r="D19" s="58"/>
-      <c r="E19" s="50"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="50"/>
+      <c r="A19" s="65"/>
+      <c r="B19" s="65"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="65"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="65"/>
       <c r="H19" s="26">
         <v>0.14255000000000001</v>
       </c>
@@ -4496,25 +4491,25 @@
       </c>
     </row>
     <row r="20" spans="1:57" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B20" s="55" t="s">
+      <c r="B20" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="C20" s="49" t="s">
+      <c r="C20" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D20" s="49" t="s">
+      <c r="D20" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="E20" s="51" t="s">
+      <c r="E20" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F20" s="49" t="s">
+      <c r="F20" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="G20" s="49" t="s">
+      <c r="G20" s="66" t="s">
         <v>55</v>
       </c>
       <c r="H20" s="17">
@@ -4669,13 +4664,13 @@
       </c>
     </row>
     <row r="21" spans="1:57" x14ac:dyDescent="0.45">
-      <c r="A21" s="59"/>
-      <c r="B21" s="53"/>
-      <c r="C21" s="44"/>
-      <c r="D21" s="44"/>
-      <c r="E21" s="44"/>
-      <c r="F21" s="44"/>
-      <c r="G21" s="44"/>
+      <c r="A21" s="77"/>
+      <c r="B21" s="75"/>
+      <c r="C21" s="64"/>
+      <c r="D21" s="64"/>
+      <c r="E21" s="64"/>
+      <c r="F21" s="64"/>
+      <c r="G21" s="64"/>
       <c r="H21" s="2">
         <v>0.18496000000000001</v>
       </c>
@@ -4828,13 +4823,13 @@
       </c>
     </row>
     <row r="22" spans="1:57" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="60"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="50"/>
-      <c r="D22" s="50"/>
-      <c r="E22" s="50"/>
-      <c r="F22" s="50"/>
-      <c r="G22" s="50"/>
+      <c r="A22" s="78"/>
+      <c r="B22" s="80"/>
+      <c r="C22" s="65"/>
+      <c r="D22" s="65"/>
+      <c r="E22" s="65"/>
+      <c r="F22" s="65"/>
+      <c r="G22" s="65"/>
       <c r="H22" s="26">
         <v>0.18983</v>
       </c>
@@ -4987,25 +4982,25 @@
       </c>
     </row>
     <row r="23" spans="1:57" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="46" t="s">
+      <c r="A23" s="60" t="s">
         <v>36</v>
       </c>
-      <c r="B23" s="51" t="s">
+      <c r="B23" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C23" s="52" t="s">
+      <c r="C23" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D23" s="49" t="s">
+      <c r="D23" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="E23" s="51" t="s">
+      <c r="E23" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F23" s="49" t="s">
+      <c r="F23" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="G23" s="49" t="s">
+      <c r="G23" s="66" t="s">
         <v>55</v>
       </c>
       <c r="H23" s="17">
@@ -5160,13 +5155,13 @@
       </c>
     </row>
     <row r="24" spans="1:57" x14ac:dyDescent="0.45">
-      <c r="A24" s="59"/>
-      <c r="B24" s="44"/>
-      <c r="C24" s="53"/>
-      <c r="D24" s="44"/>
-      <c r="E24" s="44"/>
-      <c r="F24" s="44"/>
-      <c r="G24" s="44"/>
+      <c r="A24" s="77"/>
+      <c r="B24" s="64"/>
+      <c r="C24" s="75"/>
+      <c r="D24" s="64"/>
+      <c r="E24" s="64"/>
+      <c r="F24" s="64"/>
+      <c r="G24" s="64"/>
       <c r="H24" s="2">
         <v>0.19091</v>
       </c>
@@ -5319,13 +5314,13 @@
       </c>
     </row>
     <row r="25" spans="1:57" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="60"/>
-      <c r="B25" s="50"/>
-      <c r="C25" s="54"/>
-      <c r="D25" s="50"/>
-      <c r="E25" s="50"/>
-      <c r="F25" s="50"/>
-      <c r="G25" s="50"/>
+      <c r="A25" s="78"/>
+      <c r="B25" s="65"/>
+      <c r="C25" s="80"/>
+      <c r="D25" s="65"/>
+      <c r="E25" s="65"/>
+      <c r="F25" s="65"/>
+      <c r="G25" s="65"/>
       <c r="H25" s="26">
         <v>0.20651</v>
       </c>
@@ -5481,22 +5476,22 @@
       <c r="A26" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="B26" s="51" t="s">
+      <c r="B26" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="49" t="s">
+      <c r="C26" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D26" s="55" t="s">
+      <c r="D26" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="E26" s="51" t="s">
+      <c r="E26" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F26" s="49" t="s">
+      <c r="F26" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="G26" s="51" t="s">
+      <c r="G26" s="63" t="s">
         <v>55</v>
       </c>
       <c r="H26" s="17">
@@ -5652,12 +5647,12 @@
     </row>
     <row r="27" spans="1:57" x14ac:dyDescent="0.45">
       <c r="A27" s="22"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="44"/>
-      <c r="D27" s="53"/>
-      <c r="E27" s="44"/>
-      <c r="F27" s="44"/>
-      <c r="G27" s="44"/>
+      <c r="B27" s="64"/>
+      <c r="C27" s="64"/>
+      <c r="D27" s="75"/>
+      <c r="E27" s="64"/>
+      <c r="F27" s="64"/>
+      <c r="G27" s="64"/>
       <c r="H27" s="2">
         <v>0.28672999999999998</v>
       </c>
@@ -5811,12 +5806,12 @@
     </row>
     <row r="28" spans="1:57" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="23"/>
-      <c r="B28" s="50"/>
-      <c r="C28" s="50"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="50"/>
-      <c r="F28" s="50"/>
-      <c r="G28" s="50"/>
+      <c r="B28" s="65"/>
+      <c r="C28" s="65"/>
+      <c r="D28" s="80"/>
+      <c r="E28" s="65"/>
+      <c r="F28" s="65"/>
+      <c r="G28" s="65"/>
       <c r="H28" s="26">
         <v>0.35215999999999997</v>
       </c>
@@ -5972,22 +5967,22 @@
       <c r="A29" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="B29" s="51" t="s">
+      <c r="B29" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="E29" s="55" t="s">
+      <c r="E29" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="F29" s="49" t="s">
+      <c r="F29" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="G29" s="51" t="s">
+      <c r="G29" s="63" t="s">
         <v>55</v>
       </c>
       <c r="H29" s="17">
@@ -6145,12 +6140,12 @@
       <c r="A30" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="53"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
+      <c r="B30" s="64"/>
+      <c r="C30" s="64"/>
+      <c r="D30" s="64"/>
+      <c r="E30" s="75"/>
+      <c r="F30" s="64"/>
+      <c r="G30" s="64"/>
       <c r="H30" s="2">
         <v>0.26832</v>
       </c>
@@ -6304,12 +6299,12 @@
     </row>
     <row r="31" spans="1:57" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A31" s="23"/>
-      <c r="B31" s="50"/>
-      <c r="C31" s="50"/>
-      <c r="D31" s="50"/>
-      <c r="E31" s="54"/>
-      <c r="F31" s="50"/>
-      <c r="G31" s="50"/>
+      <c r="B31" s="65"/>
+      <c r="C31" s="65"/>
+      <c r="D31" s="65"/>
+      <c r="E31" s="80"/>
+      <c r="F31" s="65"/>
+      <c r="G31" s="65"/>
       <c r="H31" s="26">
         <v>0.27560000000000001</v>
       </c>
@@ -6462,25 +6457,25 @@
       </c>
     </row>
     <row r="32" spans="1:57" s="16" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="46" t="s">
+      <c r="A32" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="B32" s="55" t="s">
+      <c r="B32" s="79" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="49" t="s">
+      <c r="C32" s="66" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="49" t="s">
+      <c r="D32" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="E32" s="55" t="s">
+      <c r="E32" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="F32" s="49" t="s">
+      <c r="F32" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="G32" s="51" t="s">
+      <c r="G32" s="63" t="s">
         <v>55</v>
       </c>
       <c r="H32" s="17">
@@ -6635,13 +6630,13 @@
       </c>
     </row>
     <row r="33" spans="1:58" x14ac:dyDescent="0.45">
-      <c r="A33" s="47"/>
-      <c r="B33" s="53"/>
-      <c r="C33" s="44"/>
-      <c r="D33" s="44"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="44"/>
-      <c r="G33" s="44"/>
+      <c r="A33" s="61"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="64"/>
+      <c r="D33" s="64"/>
+      <c r="E33" s="75"/>
+      <c r="F33" s="64"/>
+      <c r="G33" s="64"/>
       <c r="H33" s="2">
         <v>0.35682999999999998</v>
       </c>
@@ -6794,13 +6789,13 @@
       </c>
     </row>
     <row r="34" spans="1:58" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A34" s="48"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="50"/>
-      <c r="D34" s="50"/>
-      <c r="E34" s="54"/>
-      <c r="F34" s="50"/>
-      <c r="G34" s="50"/>
+      <c r="A34" s="62"/>
+      <c r="B34" s="80"/>
+      <c r="C34" s="65"/>
+      <c r="D34" s="65"/>
+      <c r="E34" s="80"/>
+      <c r="F34" s="65"/>
+      <c r="G34" s="65"/>
       <c r="H34" s="26">
         <v>0.34760000000000002</v>
       </c>
@@ -6954,16 +6949,16 @@
     </row>
     <row r="35" spans="1:58" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A35" s="15"/>
-      <c r="B35" s="51" t="s">
+      <c r="B35" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="51"/>
-      <c r="D35" s="49" t="s">
+      <c r="C35" s="63"/>
+      <c r="D35" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="51"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="51" t="s">
+      <c r="E35" s="63"/>
+      <c r="F35" s="63"/>
+      <c r="G35" s="63" t="s">
         <v>58</v>
       </c>
       <c r="H35" s="17">
@@ -7122,12 +7117,12 @@
     </row>
     <row r="36" spans="1:58" x14ac:dyDescent="0.45">
       <c r="A36" s="22"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="44"/>
-      <c r="D36" s="44"/>
-      <c r="E36" s="44"/>
-      <c r="F36" s="44"/>
-      <c r="G36" s="44"/>
+      <c r="B36" s="64"/>
+      <c r="C36" s="64"/>
+      <c r="D36" s="64"/>
+      <c r="E36" s="64"/>
+      <c r="F36" s="64"/>
+      <c r="G36" s="64"/>
       <c r="H36" s="2">
         <v>0.36908999999999997</v>
       </c>
@@ -7283,12 +7278,12 @@
       <c r="A37" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B37" s="44"/>
-      <c r="C37" s="44"/>
-      <c r="D37" s="44"/>
-      <c r="E37" s="44"/>
-      <c r="F37" s="44"/>
-      <c r="G37" s="44"/>
+      <c r="B37" s="64"/>
+      <c r="C37" s="64"/>
+      <c r="D37" s="64"/>
+      <c r="E37" s="64"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="64"/>
       <c r="H37" s="26">
         <v>0.30303999999999998</v>
       </c>
@@ -7444,12 +7439,12 @@
       <c r="A38" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="B38" s="50"/>
-      <c r="C38" s="50"/>
-      <c r="D38" s="50"/>
-      <c r="E38" s="50"/>
-      <c r="F38" s="50"/>
-      <c r="G38" s="50"/>
+      <c r="B38" s="65"/>
+      <c r="C38" s="65"/>
+      <c r="D38" s="65"/>
+      <c r="E38" s="65"/>
+      <c r="F38" s="65"/>
+      <c r="G38" s="65"/>
       <c r="H38" s="31">
         <v>0.12909000000000001</v>
       </c>
@@ -7605,16 +7600,16 @@
       <c r="A39" s="15" t="s">
         <v>50</v>
       </c>
-      <c r="B39" s="51" t="s">
+      <c r="B39" s="63" t="s">
         <v>67</v>
       </c>
-      <c r="C39" s="51"/>
-      <c r="D39" s="51" t="s">
+      <c r="C39" s="63"/>
+      <c r="D39" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="E39" s="51"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="51" t="s">
+      <c r="E39" s="63"/>
+      <c r="F39" s="63"/>
+      <c r="G39" s="63" t="s">
         <v>57</v>
       </c>
       <c r="H39" s="17">
@@ -7770,12 +7765,12 @@
     </row>
     <row r="40" spans="1:58" x14ac:dyDescent="0.45">
       <c r="A40" s="22"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="44"/>
-      <c r="D40" s="44"/>
-      <c r="E40" s="44"/>
-      <c r="F40" s="44"/>
-      <c r="G40" s="44"/>
+      <c r="B40" s="64"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="64"/>
+      <c r="E40" s="64"/>
+      <c r="F40" s="64"/>
+      <c r="G40" s="64"/>
       <c r="H40" s="2">
         <v>0.19031000000000001</v>
       </c>
@@ -7929,12 +7924,12 @@
     </row>
     <row r="41" spans="1:58" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A41" s="23"/>
-      <c r="B41" s="50"/>
-      <c r="C41" s="50"/>
-      <c r="D41" s="50"/>
-      <c r="E41" s="50"/>
-      <c r="F41" s="50"/>
-      <c r="G41" s="50"/>
+      <c r="B41" s="65"/>
+      <c r="C41" s="65"/>
+      <c r="D41" s="65"/>
+      <c r="E41" s="65"/>
+      <c r="F41" s="65"/>
+      <c r="G41" s="65"/>
       <c r="H41" s="26">
         <v>0.27665000000000001</v>
       </c>
@@ -8088,22 +8083,22 @@
     </row>
     <row r="42" spans="1:58" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A42" s="15"/>
-      <c r="B42" s="51" t="s">
+      <c r="B42" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="52" t="s">
+      <c r="C42" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D42" s="55" t="s">
+      <c r="D42" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="E42" s="51" t="s">
+      <c r="E42" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F42" s="52" t="s">
+      <c r="F42" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G42" s="51" t="s">
+      <c r="G42" s="63" t="s">
         <v>54</v>
       </c>
       <c r="H42" s="17">
@@ -8262,12 +8257,12 @@
     </row>
     <row r="43" spans="1:58" x14ac:dyDescent="0.45">
       <c r="A43" s="22"/>
-      <c r="B43" s="44"/>
-      <c r="C43" s="53"/>
-      <c r="D43" s="53"/>
-      <c r="E43" s="44"/>
-      <c r="F43" s="53"/>
-      <c r="G43" s="44"/>
+      <c r="B43" s="64"/>
+      <c r="C43" s="75"/>
+      <c r="D43" s="75"/>
+      <c r="E43" s="64"/>
+      <c r="F43" s="75"/>
+      <c r="G43" s="64"/>
       <c r="H43" s="2">
         <v>0.37514999999999998</v>
       </c>
@@ -8421,12 +8416,12 @@
     </row>
     <row r="44" spans="1:58" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A44" s="23"/>
-      <c r="B44" s="50"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="54"/>
-      <c r="E44" s="50"/>
-      <c r="F44" s="54"/>
-      <c r="G44" s="50"/>
+      <c r="B44" s="65"/>
+      <c r="C44" s="80"/>
+      <c r="D44" s="80"/>
+      <c r="E44" s="65"/>
+      <c r="F44" s="80"/>
+      <c r="G44" s="65"/>
       <c r="H44" s="26">
         <v>0.39378999999999997</v>
       </c>
@@ -8580,22 +8575,22 @@
     </row>
     <row r="45" spans="1:58" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A45" s="15"/>
-      <c r="B45" s="51" t="s">
+      <c r="B45" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C45" s="52" t="s">
+      <c r="C45" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D45" s="49" t="s">
+      <c r="D45" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="E45" s="51" t="s">
+      <c r="E45" s="63" t="s">
         <v>19</v>
       </c>
-      <c r="F45" s="52" t="s">
+      <c r="F45" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G45" s="51" t="s">
+      <c r="G45" s="63" t="s">
         <v>54</v>
       </c>
       <c r="H45" s="17">
@@ -8751,12 +8746,12 @@
     </row>
     <row r="46" spans="1:58" x14ac:dyDescent="0.45">
       <c r="A46" s="22"/>
-      <c r="B46" s="44"/>
-      <c r="C46" s="53"/>
-      <c r="D46" s="44"/>
-      <c r="E46" s="44"/>
-      <c r="F46" s="53"/>
-      <c r="G46" s="44"/>
+      <c r="B46" s="64"/>
+      <c r="C46" s="75"/>
+      <c r="D46" s="64"/>
+      <c r="E46" s="64"/>
+      <c r="F46" s="75"/>
+      <c r="G46" s="64"/>
       <c r="H46" s="2">
         <v>0.19091</v>
       </c>
@@ -8910,12 +8905,12 @@
     </row>
     <row r="47" spans="1:58" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A47" s="23"/>
-      <c r="B47" s="50"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="50"/>
-      <c r="E47" s="50"/>
-      <c r="F47" s="54"/>
-      <c r="G47" s="50"/>
+      <c r="B47" s="65"/>
+      <c r="C47" s="80"/>
+      <c r="D47" s="65"/>
+      <c r="E47" s="65"/>
+      <c r="F47" s="80"/>
+      <c r="G47" s="65"/>
       <c r="H47" s="26">
         <v>0.19620000000000001</v>
       </c>
@@ -9069,22 +9064,22 @@
     </row>
     <row r="48" spans="1:58" s="16" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A48" s="15"/>
-      <c r="B48" s="51" t="s">
+      <c r="B48" s="63" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="52" t="s">
+      <c r="C48" s="81" t="s">
         <v>21</v>
       </c>
-      <c r="D48" s="49" t="s">
+      <c r="D48" s="66" t="s">
         <v>0</v>
       </c>
-      <c r="E48" s="55" t="s">
+      <c r="E48" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="F48" s="52" t="s">
+      <c r="F48" s="81" t="s">
         <v>25</v>
       </c>
-      <c r="G48" s="51" t="s">
+      <c r="G48" s="63" t="s">
         <v>54</v>
       </c>
       <c r="H48" s="17">
@@ -9240,12 +9235,12 @@
     </row>
     <row r="49" spans="1:57" x14ac:dyDescent="0.45">
       <c r="A49" s="22"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="53"/>
-      <c r="D49" s="44"/>
-      <c r="E49" s="53"/>
-      <c r="F49" s="53"/>
-      <c r="G49" s="44"/>
+      <c r="B49" s="64"/>
+      <c r="C49" s="75"/>
+      <c r="D49" s="64"/>
+      <c r="E49" s="75"/>
+      <c r="F49" s="75"/>
+      <c r="G49" s="64"/>
       <c r="H49" s="2">
         <v>0.29293999999999998</v>
       </c>
@@ -9399,12 +9394,12 @@
     </row>
     <row r="50" spans="1:57" s="24" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A50" s="23"/>
-      <c r="B50" s="50"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="50"/>
-      <c r="E50" s="54"/>
-      <c r="F50" s="54"/>
-      <c r="G50" s="50"/>
+      <c r="B50" s="65"/>
+      <c r="C50" s="80"/>
+      <c r="D50" s="65"/>
+      <c r="E50" s="80"/>
+      <c r="F50" s="80"/>
+      <c r="G50" s="65"/>
       <c r="H50" s="26">
         <v>0.31709999999999999</v>
       </c>
@@ -9558,28 +9553,28 @@
     </row>
     <row r="51" spans="1:57" ht="14" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A51" s="14"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="45"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="44"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="44"/>
+      <c r="B51" s="64"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="67"/>
+      <c r="E51" s="64"/>
+      <c r="F51" s="64"/>
+      <c r="G51" s="64"/>
     </row>
     <row r="52" spans="1:57" x14ac:dyDescent="0.45">
-      <c r="B52" s="44"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="45"/>
-      <c r="E52" s="44"/>
-      <c r="F52" s="44"/>
-      <c r="G52" s="44"/>
+      <c r="B52" s="64"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="67"/>
+      <c r="E52" s="64"/>
+      <c r="F52" s="64"/>
+      <c r="G52" s="64"/>
     </row>
     <row r="53" spans="1:57" x14ac:dyDescent="0.45">
-      <c r="B53" s="44"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="44"/>
-      <c r="F53" s="44"/>
-      <c r="G53" s="44"/>
+      <c r="B53" s="64"/>
+      <c r="C53" s="67"/>
+      <c r="D53" s="67"/>
+      <c r="E53" s="64"/>
+      <c r="F53" s="64"/>
+      <c r="G53" s="64"/>
     </row>
     <row r="55" spans="1:57" x14ac:dyDescent="0.45">
       <c r="B55" s="14" t="s">
@@ -9597,7 +9592,7 @@
       </c>
     </row>
     <row r="61" spans="1:57" x14ac:dyDescent="0.45">
-      <c r="H61" s="73" t="s">
+      <c r="H61" s="47" t="s">
         <v>118</v>
       </c>
       <c r="J61" s="14" t="s">
@@ -9699,30 +9694,76 @@
         <v>1385.9690000000001</v>
       </c>
     </row>
+    <row r="67" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="H67" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="J67" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="68" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="I68" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K68" s="1">
+        <v>17114</v>
+      </c>
+      <c r="M68" s="5" t="s">
+        <v>150</v>
+      </c>
+      <c r="O68" s="1">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="69" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K69" s="1">
+        <v>17356</v>
+      </c>
+      <c r="O69" s="1">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="70" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K70" s="1">
+        <v>16787</v>
+      </c>
+      <c r="O70" s="1">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="71" spans="1:15" x14ac:dyDescent="0.45">
+      <c r="K71" s="1">
+        <v>17083</v>
+      </c>
+      <c r="O71" s="1">
+        <v>76</v>
+      </c>
+    </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A78" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B78" s="44" t="s">
+      <c r="B78" s="64" t="s">
         <v>76</v>
       </c>
-      <c r="C78" s="44"/>
-      <c r="D78" s="44" t="s">
+      <c r="C78" s="64"/>
+      <c r="D78" s="64" t="s">
         <v>77</v>
       </c>
-      <c r="E78" s="44"/>
-      <c r="F78" s="44" t="s">
+      <c r="E78" s="64"/>
+      <c r="F78" s="64" t="s">
         <v>78</v>
       </c>
-      <c r="G78" s="57"/>
-      <c r="H78" s="56" t="s">
+      <c r="G78" s="73"/>
+      <c r="H78" s="72" t="s">
         <v>79</v>
       </c>
-      <c r="I78" s="44"/>
-      <c r="J78" s="44" t="s">
+      <c r="I78" s="64"/>
+      <c r="J78" s="64" t="s">
         <v>80</v>
       </c>
-      <c r="K78" s="44"/>
+      <c r="K78" s="64"/>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.45">
       <c r="B79" s="1" t="s">
@@ -10388,27 +10429,85 @@
     </row>
   </sheetData>
   <mergeCells count="124">
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C4:C8"/>
-    <mergeCell ref="D4:D8"/>
-    <mergeCell ref="E4:E8"/>
-    <mergeCell ref="F4:F8"/>
-    <mergeCell ref="G4:G8"/>
-    <mergeCell ref="A17:A19"/>
-    <mergeCell ref="R1:AA1"/>
-    <mergeCell ref="R2:V2"/>
-    <mergeCell ref="X2:AA2"/>
-    <mergeCell ref="B11:B13"/>
-    <mergeCell ref="C11:C13"/>
-    <mergeCell ref="A11:A13"/>
-    <mergeCell ref="D14:D16"/>
-    <mergeCell ref="E14:E16"/>
-    <mergeCell ref="D11:D13"/>
-    <mergeCell ref="E11:E13"/>
-    <mergeCell ref="F11:F13"/>
-    <mergeCell ref="H1:Q1"/>
-    <mergeCell ref="A14:A16"/>
+    <mergeCell ref="B51:B53"/>
+    <mergeCell ref="C51:C53"/>
+    <mergeCell ref="D51:D53"/>
+    <mergeCell ref="E51:E53"/>
+    <mergeCell ref="F51:F53"/>
+    <mergeCell ref="G51:G53"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="B45:B47"/>
+    <mergeCell ref="F32:F34"/>
+    <mergeCell ref="D35:D38"/>
+    <mergeCell ref="G42:G44"/>
+    <mergeCell ref="F42:F44"/>
+    <mergeCell ref="E42:E44"/>
+    <mergeCell ref="D42:D44"/>
+    <mergeCell ref="F35:F38"/>
+    <mergeCell ref="E35:E38"/>
+    <mergeCell ref="G39:G41"/>
+    <mergeCell ref="F39:F41"/>
+    <mergeCell ref="E39:E41"/>
+    <mergeCell ref="D39:D41"/>
+    <mergeCell ref="D32:D34"/>
+    <mergeCell ref="G35:G38"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="AB1:AK1"/>
+    <mergeCell ref="AB2:AF2"/>
+    <mergeCell ref="G20:G22"/>
+    <mergeCell ref="G11:G13"/>
+    <mergeCell ref="G14:G16"/>
+    <mergeCell ref="G23:G25"/>
+    <mergeCell ref="C23:C25"/>
+    <mergeCell ref="B14:B16"/>
+    <mergeCell ref="C14:C16"/>
+    <mergeCell ref="C20:C22"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B20:B22"/>
+    <mergeCell ref="E23:E25"/>
+    <mergeCell ref="D23:D25"/>
+    <mergeCell ref="AH2:AK2"/>
+    <mergeCell ref="H2:L2"/>
+    <mergeCell ref="N2:Q2"/>
+    <mergeCell ref="F14:F16"/>
+    <mergeCell ref="B17:B19"/>
+    <mergeCell ref="C17:C19"/>
+    <mergeCell ref="D17:D19"/>
+    <mergeCell ref="E17:E19"/>
+    <mergeCell ref="F17:F19"/>
+    <mergeCell ref="G17:G19"/>
+    <mergeCell ref="BL1:BL3"/>
+    <mergeCell ref="AL1:AU1"/>
+    <mergeCell ref="AL2:AP2"/>
+    <mergeCell ref="AR2:AU2"/>
+    <mergeCell ref="AV1:BE1"/>
+    <mergeCell ref="AV2:AZ2"/>
+    <mergeCell ref="BB2:BE2"/>
+    <mergeCell ref="BG1:BG3"/>
+    <mergeCell ref="BH1:BH3"/>
+    <mergeCell ref="BI1:BI3"/>
+    <mergeCell ref="BJ1:BJ3"/>
+    <mergeCell ref="BK1:BK3"/>
+    <mergeCell ref="BF1:BF3"/>
+    <mergeCell ref="G29:G31"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="E26:E28"/>
+    <mergeCell ref="F26:F28"/>
+    <mergeCell ref="E29:E31"/>
+    <mergeCell ref="D29:D31"/>
+    <mergeCell ref="F29:F31"/>
+    <mergeCell ref="A23:A25"/>
+    <mergeCell ref="A20:A22"/>
+    <mergeCell ref="D20:D22"/>
+    <mergeCell ref="F23:F25"/>
+    <mergeCell ref="E20:E22"/>
+    <mergeCell ref="F20:F22"/>
+    <mergeCell ref="B26:B28"/>
+    <mergeCell ref="G26:G28"/>
+    <mergeCell ref="B29:B31"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="C29:C31"/>
     <mergeCell ref="E32:E34"/>
     <mergeCell ref="B32:B34"/>
     <mergeCell ref="B78:C78"/>
@@ -10433,85 +10532,27 @@
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="C42:C44"/>
     <mergeCell ref="B42:B44"/>
-    <mergeCell ref="G29:G31"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="E26:E28"/>
-    <mergeCell ref="F26:F28"/>
-    <mergeCell ref="E29:E31"/>
-    <mergeCell ref="D29:D31"/>
-    <mergeCell ref="F29:F31"/>
-    <mergeCell ref="A23:A25"/>
-    <mergeCell ref="A20:A22"/>
-    <mergeCell ref="D20:D22"/>
-    <mergeCell ref="F23:F25"/>
-    <mergeCell ref="E20:E22"/>
-    <mergeCell ref="F20:F22"/>
-    <mergeCell ref="B26:B28"/>
-    <mergeCell ref="G26:G28"/>
-    <mergeCell ref="B29:B31"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="C29:C31"/>
-    <mergeCell ref="BL1:BL3"/>
-    <mergeCell ref="AL1:AU1"/>
-    <mergeCell ref="AL2:AP2"/>
-    <mergeCell ref="AR2:AU2"/>
-    <mergeCell ref="AV1:BE1"/>
-    <mergeCell ref="AV2:AZ2"/>
-    <mergeCell ref="BB2:BE2"/>
-    <mergeCell ref="BG1:BG3"/>
-    <mergeCell ref="BH1:BH3"/>
-    <mergeCell ref="BI1:BI3"/>
-    <mergeCell ref="BJ1:BJ3"/>
-    <mergeCell ref="BK1:BK3"/>
-    <mergeCell ref="BF1:BF3"/>
-    <mergeCell ref="AB1:AK1"/>
-    <mergeCell ref="AB2:AF2"/>
-    <mergeCell ref="G20:G22"/>
-    <mergeCell ref="G11:G13"/>
-    <mergeCell ref="G14:G16"/>
-    <mergeCell ref="G23:G25"/>
-    <mergeCell ref="C23:C25"/>
-    <mergeCell ref="B14:B16"/>
-    <mergeCell ref="C14:C16"/>
-    <mergeCell ref="C20:C22"/>
-    <mergeCell ref="B23:B25"/>
-    <mergeCell ref="B20:B22"/>
-    <mergeCell ref="E23:E25"/>
-    <mergeCell ref="D23:D25"/>
-    <mergeCell ref="AH2:AK2"/>
-    <mergeCell ref="H2:L2"/>
-    <mergeCell ref="N2:Q2"/>
-    <mergeCell ref="F14:F16"/>
-    <mergeCell ref="B17:B19"/>
-    <mergeCell ref="C17:C19"/>
-    <mergeCell ref="D17:D19"/>
-    <mergeCell ref="E17:E19"/>
-    <mergeCell ref="F17:F19"/>
-    <mergeCell ref="G17:G19"/>
-    <mergeCell ref="B51:B53"/>
-    <mergeCell ref="C51:C53"/>
-    <mergeCell ref="D51:D53"/>
-    <mergeCell ref="E51:E53"/>
-    <mergeCell ref="F51:F53"/>
-    <mergeCell ref="G51:G53"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="B45:B47"/>
-    <mergeCell ref="F32:F34"/>
-    <mergeCell ref="D35:D38"/>
-    <mergeCell ref="G42:G44"/>
-    <mergeCell ref="F42:F44"/>
-    <mergeCell ref="E42:E44"/>
-    <mergeCell ref="D42:D44"/>
-    <mergeCell ref="F35:F38"/>
-    <mergeCell ref="E35:E38"/>
-    <mergeCell ref="G39:G41"/>
-    <mergeCell ref="F39:F41"/>
-    <mergeCell ref="E39:E41"/>
-    <mergeCell ref="D39:D41"/>
-    <mergeCell ref="D32:D34"/>
-    <mergeCell ref="G35:G38"/>
-    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="C4:C8"/>
+    <mergeCell ref="D4:D8"/>
+    <mergeCell ref="E4:E8"/>
+    <mergeCell ref="F4:F8"/>
+    <mergeCell ref="G4:G8"/>
+    <mergeCell ref="A17:A19"/>
+    <mergeCell ref="R1:AA1"/>
+    <mergeCell ref="R2:V2"/>
+    <mergeCell ref="X2:AA2"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="C11:C13"/>
+    <mergeCell ref="A11:A13"/>
+    <mergeCell ref="D14:D16"/>
+    <mergeCell ref="E14:E16"/>
+    <mergeCell ref="D11:D13"/>
+    <mergeCell ref="E11:E13"/>
+    <mergeCell ref="F11:F13"/>
+    <mergeCell ref="H1:Q1"/>
+    <mergeCell ref="A14:A16"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B80:B93">
@@ -10640,10 +10681,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{786D7229-4A72-4AE9-B9C9-5C6ADD0B8395}">
-  <dimension ref="A1:BY45"/>
+  <dimension ref="A1:BY52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="K46" sqref="K46"/>
+    <sheetView topLeftCell="A20" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H45" sqref="H45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.45"/>
@@ -10656,8 +10697,7 @@
     <col min="16" max="27" width="8.9375" style="1"/>
     <col min="28" max="28" width="8.9375" style="37"/>
     <col min="29" max="29" width="8.9375" style="3"/>
-    <col min="30" max="30" width="8.9375" style="74"/>
-    <col min="31" max="41" width="8.9375" style="1"/>
+    <col min="30" max="41" width="8.9375" style="1"/>
     <col min="42" max="42" width="8.9375" style="37"/>
     <col min="43" max="43" width="8.9375" style="3"/>
     <col min="44" max="44" width="8.9375" style="2"/>
@@ -10666,9 +10706,9 @@
     <col min="57" max="57" width="8.9375" style="3"/>
     <col min="58" max="58" width="8.9375" style="2"/>
     <col min="59" max="67" width="8.9375" style="1"/>
-    <col min="68" max="68" width="8.9375" style="78"/>
-    <col min="69" max="69" width="8.9375" style="74"/>
-    <col min="70" max="70" width="8.9375" style="76"/>
+    <col min="68" max="68" width="8.9375" style="6"/>
+    <col min="69" max="69" width="8.9375" style="1"/>
+    <col min="70" max="70" width="8.9375" style="37"/>
     <col min="71" max="71" width="8.9375" style="3"/>
     <col min="72" max="76" width="8.9375" style="1"/>
     <col min="77" max="77" width="8.9375" style="14"/>
@@ -10676,86 +10716,86 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:77" x14ac:dyDescent="0.45">
-      <c r="B1" s="56" t="s">
+      <c r="B1" s="72" t="s">
         <v>96</v>
       </c>
-      <c r="C1" s="44"/>
-      <c r="D1" s="44"/>
-      <c r="E1" s="44"/>
-      <c r="F1" s="44"/>
-      <c r="G1" s="44"/>
-      <c r="H1" s="44"/>
-      <c r="I1" s="44"/>
-      <c r="J1" s="44"/>
-      <c r="K1" s="44"/>
-      <c r="L1" s="44"/>
-      <c r="M1" s="44"/>
-      <c r="N1" s="44"/>
-      <c r="O1" s="57"/>
-      <c r="P1" s="44" t="s">
+      <c r="C1" s="64"/>
+      <c r="D1" s="64"/>
+      <c r="E1" s="64"/>
+      <c r="F1" s="64"/>
+      <c r="G1" s="64"/>
+      <c r="H1" s="64"/>
+      <c r="I1" s="64"/>
+      <c r="J1" s="64"/>
+      <c r="K1" s="64"/>
+      <c r="L1" s="64"/>
+      <c r="M1" s="64"/>
+      <c r="N1" s="64"/>
+      <c r="O1" s="73"/>
+      <c r="P1" s="64" t="s">
         <v>97</v>
       </c>
-      <c r="Q1" s="44"/>
-      <c r="R1" s="44"/>
-      <c r="S1" s="44"/>
-      <c r="T1" s="44"/>
-      <c r="U1" s="44"/>
-      <c r="V1" s="44"/>
-      <c r="W1" s="44"/>
-      <c r="X1" s="44"/>
-      <c r="Y1" s="44"/>
-      <c r="Z1" s="44"/>
-      <c r="AA1" s="44"/>
-      <c r="AB1" s="44"/>
-      <c r="AC1" s="44"/>
-      <c r="AD1" s="56" t="s">
+      <c r="Q1" s="64"/>
+      <c r="R1" s="64"/>
+      <c r="S1" s="64"/>
+      <c r="T1" s="64"/>
+      <c r="U1" s="64"/>
+      <c r="V1" s="64"/>
+      <c r="W1" s="64"/>
+      <c r="X1" s="64"/>
+      <c r="Y1" s="64"/>
+      <c r="Z1" s="64"/>
+      <c r="AA1" s="64"/>
+      <c r="AB1" s="64"/>
+      <c r="AC1" s="64"/>
+      <c r="AD1" s="72" t="s">
         <v>103</v>
       </c>
-      <c r="AE1" s="44"/>
-      <c r="AF1" s="44"/>
-      <c r="AG1" s="44"/>
-      <c r="AH1" s="44"/>
-      <c r="AI1" s="44"/>
-      <c r="AJ1" s="44"/>
-      <c r="AK1" s="44"/>
-      <c r="AL1" s="44"/>
-      <c r="AM1" s="44"/>
-      <c r="AN1" s="44"/>
-      <c r="AO1" s="44"/>
-      <c r="AP1" s="44"/>
-      <c r="AQ1" s="57"/>
-      <c r="AR1" s="56" t="s">
+      <c r="AE1" s="64"/>
+      <c r="AF1" s="64"/>
+      <c r="AG1" s="64"/>
+      <c r="AH1" s="64"/>
+      <c r="AI1" s="64"/>
+      <c r="AJ1" s="64"/>
+      <c r="AK1" s="64"/>
+      <c r="AL1" s="64"/>
+      <c r="AM1" s="64"/>
+      <c r="AN1" s="64"/>
+      <c r="AO1" s="64"/>
+      <c r="AP1" s="64"/>
+      <c r="AQ1" s="73"/>
+      <c r="AR1" s="72" t="s">
         <v>98</v>
       </c>
-      <c r="AS1" s="44"/>
-      <c r="AT1" s="44"/>
-      <c r="AU1" s="44"/>
-      <c r="AV1" s="44"/>
-      <c r="AW1" s="44"/>
-      <c r="AX1" s="44"/>
-      <c r="AY1" s="44"/>
-      <c r="AZ1" s="44"/>
-      <c r="BA1" s="44"/>
-      <c r="BB1" s="44"/>
-      <c r="BC1" s="44"/>
-      <c r="BD1" s="44"/>
-      <c r="BE1" s="57"/>
-      <c r="BF1" s="56" t="s">
+      <c r="AS1" s="64"/>
+      <c r="AT1" s="64"/>
+      <c r="AU1" s="64"/>
+      <c r="AV1" s="64"/>
+      <c r="AW1" s="64"/>
+      <c r="AX1" s="64"/>
+      <c r="AY1" s="64"/>
+      <c r="AZ1" s="64"/>
+      <c r="BA1" s="64"/>
+      <c r="BB1" s="64"/>
+      <c r="BC1" s="64"/>
+      <c r="BD1" s="64"/>
+      <c r="BE1" s="73"/>
+      <c r="BF1" s="72" t="s">
         <v>99</v>
       </c>
-      <c r="BG1" s="44"/>
-      <c r="BH1" s="44"/>
-      <c r="BI1" s="44"/>
-      <c r="BJ1" s="44"/>
-      <c r="BK1" s="44"/>
-      <c r="BL1" s="44"/>
-      <c r="BM1" s="44"/>
-      <c r="BN1" s="44"/>
-      <c r="BO1" s="44"/>
-      <c r="BP1" s="44"/>
-      <c r="BQ1" s="44"/>
-      <c r="BR1" s="44"/>
-      <c r="BS1" s="57"/>
+      <c r="BG1" s="64"/>
+      <c r="BH1" s="64"/>
+      <c r="BI1" s="64"/>
+      <c r="BJ1" s="64"/>
+      <c r="BK1" s="64"/>
+      <c r="BL1" s="64"/>
+      <c r="BM1" s="64"/>
+      <c r="BN1" s="64"/>
+      <c r="BO1" s="64"/>
+      <c r="BP1" s="64"/>
+      <c r="BQ1" s="64"/>
+      <c r="BR1" s="64"/>
+      <c r="BS1" s="73"/>
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
@@ -10845,7 +10885,7 @@
       <c r="AC3" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="AD3" s="74" t="s">
+      <c r="AD3" s="1" t="s">
         <v>13</v>
       </c>
       <c r="AE3" s="1" t="s">
@@ -10959,13 +10999,13 @@
       <c r="BO3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="BP3" s="78" t="s">
+      <c r="BP3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="BQ3" s="74" t="s">
+      <c r="BQ3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="BR3" s="76" t="s">
+      <c r="BR3" s="37" t="s">
         <v>5</v>
       </c>
       <c r="BS3" s="3" t="s">
@@ -11040,7 +11080,7 @@
       </c>
       <c r="AB4" s="40"/>
       <c r="AC4" s="41"/>
-      <c r="AD4" s="75">
+      <c r="AD4" s="38">
         <v>0.27006802721088402</v>
       </c>
       <c r="AE4" s="38">
@@ -11134,9 +11174,8 @@
       <c r="BO4" s="38">
         <v>0.67522249018895297</v>
       </c>
-      <c r="BP4" s="87"/>
-      <c r="BQ4" s="75"/>
-      <c r="BR4" s="77"/>
+      <c r="BP4" s="54"/>
+      <c r="BR4" s="40"/>
       <c r="BS4" s="41"/>
       <c r="BT4" s="38" t="s">
         <v>104</v>
@@ -11153,10 +11192,10 @@
       <c r="BX4" s="38" t="s">
         <v>108</v>
       </c>
-      <c r="BY4" s="70"/>
+      <c r="BY4" s="44"/>
     </row>
     <row r="5" spans="1:77" x14ac:dyDescent="0.45">
-      <c r="A5" s="63" t="s">
+      <c r="A5" s="70" t="s">
         <v>112</v>
       </c>
       <c r="L5" s="1">
@@ -11207,13 +11246,13 @@
       <c r="BE5" s="1">
         <v>0.66913139746667205</v>
       </c>
-      <c r="BP5" s="78">
+      <c r="BP5" s="6">
         <v>0.62736062040194696</v>
       </c>
-      <c r="BQ5" s="74">
+      <c r="BQ5" s="1">
         <v>0.61989079414890902</v>
       </c>
-      <c r="BR5" s="76">
+      <c r="BR5" s="37">
         <v>0.60309377370790995</v>
       </c>
       <c r="BS5" s="3">
@@ -11241,7 +11280,7 @@
       </c>
     </row>
     <row r="6" spans="1:77" x14ac:dyDescent="0.45">
-      <c r="A6" s="57"/>
+      <c r="A6" s="73"/>
       <c r="L6" s="1">
         <v>0.80758926741580805</v>
       </c>
@@ -11266,7 +11305,6 @@
       <c r="AC6" s="3">
         <v>0.78279138736772103</v>
       </c>
-      <c r="AD6" s="1"/>
       <c r="AN6" s="1">
         <v>0.67844702773738697</v>
       </c>
@@ -11291,13 +11329,13 @@
       <c r="BE6" s="1">
         <v>0.66841426678381699</v>
       </c>
-      <c r="BP6" s="78">
+      <c r="BP6" s="6">
         <v>0.62516782311953201</v>
       </c>
-      <c r="BQ6" s="74">
+      <c r="BQ6" s="1">
         <v>0.61739458505531597</v>
       </c>
-      <c r="BR6" s="76">
+      <c r="BR6" s="37">
         <v>0.60141252271308898</v>
       </c>
       <c r="BS6" s="3">
@@ -11325,7 +11363,7 @@
       </c>
     </row>
     <row r="7" spans="1:77" x14ac:dyDescent="0.45">
-      <c r="A7" s="67"/>
+      <c r="A7" s="83"/>
       <c r="L7" s="1">
         <v>0.80552627469246996</v>
       </c>
@@ -11374,13 +11412,13 @@
       <c r="BE7" s="1">
         <v>0.67057473970968695</v>
       </c>
-      <c r="BP7" s="78">
+      <c r="BP7" s="6">
         <v>0.62837393593443003</v>
       </c>
-      <c r="BQ7" s="74">
+      <c r="BQ7" s="1">
         <v>0.62010084679189803</v>
       </c>
-      <c r="BR7" s="76">
+      <c r="BR7" s="37">
         <v>0.60573431126551502</v>
       </c>
       <c r="BS7" s="3">
@@ -11408,7 +11446,7 @@
       </c>
     </row>
     <row r="8" spans="1:77" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="68" t="s">
+      <c r="A8" s="84" t="s">
         <v>111</v>
       </c>
       <c r="B8" s="17"/>
@@ -11494,68 +11532,65 @@
         <f>BR8/$BN$4</f>
         <v>0.76777023253493715</v>
       </c>
-      <c r="BY8" s="71"/>
+      <c r="BY8" s="45"/>
     </row>
-    <row r="9" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="69"/>
-      <c r="B9" s="2"/>
-      <c r="L9" s="74">
+    <row r="9" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A9" s="85"/>
+      <c r="L9" s="1">
         <v>0.81310560079151795</v>
       </c>
-      <c r="M9" s="74">
+      <c r="M9" s="1">
         <v>0.88869719743817599</v>
       </c>
-      <c r="N9" s="76">
+      <c r="N9" s="37">
         <v>0.84558677830789297</v>
       </c>
       <c r="O9" s="3">
         <v>0.78484278445409095</v>
       </c>
-      <c r="Z9" s="74">
+      <c r="Z9" s="1">
         <v>0.76371502719879303</v>
       </c>
-      <c r="AA9" s="74">
+      <c r="AA9" s="1">
         <v>0.84404734295153705</v>
       </c>
-      <c r="AB9" s="76">
+      <c r="AB9" s="37">
         <v>0.79801591334955702</v>
       </c>
       <c r="AC9" s="3">
         <v>0.78282349393361805</v>
       </c>
-      <c r="AN9" s="74">
+      <c r="AN9" s="1">
         <v>0.68817412624264296</v>
       </c>
-      <c r="AO9" s="74">
+      <c r="AO9" s="1">
         <v>0.771872706994993</v>
       </c>
-      <c r="AP9" s="76">
+      <c r="AP9" s="37">
         <v>0.72243528451876105</v>
       </c>
-      <c r="AQ9" s="74">
+      <c r="AQ9" s="1">
         <v>0.79590925361680298</v>
       </c>
-      <c r="AR9" s="2"/>
-      <c r="BB9" s="74">
+      <c r="BB9" s="1">
         <v>0.65388179465181495</v>
       </c>
-      <c r="BC9" s="74">
+      <c r="BC9" s="1">
         <v>0.71807792744013699</v>
       </c>
-      <c r="BD9" s="76">
+      <c r="BD9" s="37">
         <v>0.66554799938155396</v>
       </c>
-      <c r="BE9" s="74">
+      <c r="BE9" s="1">
         <v>0.67057100291673799</v>
       </c>
-      <c r="BF9" s="2"/>
-      <c r="BP9" s="78">
+      <c r="BP9" s="6">
         <v>0.62372946519066996</v>
       </c>
-      <c r="BQ9" s="74">
+      <c r="BQ9" s="1">
         <v>0.61931110577702597</v>
       </c>
-      <c r="BR9" s="76">
+      <c r="BR9" s="37">
         <v>0.60356583052608304</v>
       </c>
       <c r="BS9" s="3">
@@ -11581,68 +11616,64 @@
         <f t="shared" ref="BX9" si="9">BR9/$BN$4</f>
         <v>0.77660404732036525</v>
       </c>
-      <c r="BY9" s="79"/>
     </row>
-    <row r="10" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="69"/>
-      <c r="B10" s="2"/>
-      <c r="L10" s="74">
+    <row r="10" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A10" s="85"/>
+      <c r="L10" s="1">
         <v>0.81192925389801496</v>
       </c>
-      <c r="M10" s="74">
+      <c r="M10" s="1">
         <v>0.88782452179520899</v>
       </c>
-      <c r="N10" s="76">
+      <c r="N10" s="37">
         <v>0.84462859869432605</v>
       </c>
       <c r="O10" s="3">
         <v>0.78471423564647003</v>
       </c>
-      <c r="Z10" s="74">
+      <c r="Z10" s="1">
         <v>0.76367424058147104</v>
       </c>
-      <c r="AA10" s="74">
+      <c r="AA10" s="1">
         <v>0.84621708379504301</v>
       </c>
-      <c r="AB10" s="76">
+      <c r="AB10" s="37">
         <v>0.79922105642691799</v>
       </c>
       <c r="AC10" s="3">
         <v>0.78254469295060203</v>
       </c>
-      <c r="AN10" s="74">
+      <c r="AN10" s="1">
         <v>0.69169877961786796</v>
       </c>
-      <c r="AO10" s="74">
+      <c r="AO10" s="1">
         <v>0.77224950167825201</v>
       </c>
-      <c r="AP10" s="76">
+      <c r="AP10" s="37">
         <v>0.72357701264484198</v>
       </c>
-      <c r="AQ10" s="74">
+      <c r="AQ10" s="1">
         <v>0.79492970724927703</v>
       </c>
-      <c r="AR10" s="2"/>
-      <c r="BB10" s="74">
+      <c r="BB10" s="1">
         <v>0.66175349260406502</v>
       </c>
-      <c r="BC10" s="74">
+      <c r="BC10" s="1">
         <v>0.72722601701607104</v>
       </c>
-      <c r="BD10" s="76">
+      <c r="BD10" s="37">
         <v>0.67837312942240102</v>
       </c>
-      <c r="BE10" s="74">
+      <c r="BE10" s="1">
         <v>0.670351853492266</v>
       </c>
-      <c r="BF10" s="2"/>
-      <c r="BP10" s="78">
+      <c r="BP10" s="6">
         <v>0.63433273355978503</v>
       </c>
-      <c r="BQ10" s="74">
+      <c r="BQ10" s="1">
         <v>0.62944785515008295</v>
       </c>
-      <c r="BR10" s="76">
+      <c r="BR10" s="37">
         <v>0.61394918278816102</v>
       </c>
       <c r="BS10" s="3">
@@ -11668,12 +11699,12 @@
         <f t="shared" ref="BX10" si="14">BR10/$BN$4</f>
         <v>0.78996423602497479</v>
       </c>
-      <c r="BY10" s="79" t="s">
+      <c r="BY10" s="14" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="11" spans="1:77" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A11" s="80"/>
+      <c r="A11" s="86"/>
       <c r="B11" s="26"/>
       <c r="L11" s="24">
         <v>0.81259755653468202</v>
@@ -11737,121 +11768,118 @@
       <c r="BS11" s="25">
         <v>0.66530512918148099</v>
       </c>
-      <c r="BT11" s="81">
+      <c r="BT11" s="48">
         <f>N11/$J$4</f>
         <v>0.98952210842747113</v>
       </c>
-      <c r="BU11" s="81">
+      <c r="BU11" s="48">
         <f>AB11/$X$4</f>
         <v>0.96389894493546446</v>
       </c>
-      <c r="BV11" s="81">
+      <c r="BV11" s="48">
         <f>AP11/$AL$4</f>
         <v>0.91735514987562061</v>
       </c>
-      <c r="BW11" s="81">
+      <c r="BW11" s="48">
         <f>BD11/$AZ$4</f>
         <v>0.82796423254103502</v>
       </c>
-      <c r="BX11" s="81">
+      <c r="BX11" s="48">
         <f>BR11/$BN$4</f>
         <v>0.77630982110222757</v>
       </c>
-      <c r="BY11" s="72"/>
+      <c r="BY11" s="46"/>
     </row>
-    <row r="12" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A12" s="62" t="s">
+    <row r="12" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A12" s="69" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="2"/>
-      <c r="L12" s="74">
+      <c r="L12" s="1">
         <v>0.81316840370401999</v>
       </c>
-      <c r="M12" s="74">
+      <c r="M12" s="1">
         <v>0.89030947538838801</v>
       </c>
-      <c r="N12" s="76">
+      <c r="N12" s="37">
         <v>0.84664689275348604</v>
       </c>
       <c r="O12" s="3">
         <v>0.78479596656972594</v>
       </c>
-      <c r="Z12" s="74">
+      <c r="Z12" s="1">
         <v>0.763359194436391</v>
       </c>
-      <c r="AA12" s="74">
+      <c r="AA12" s="1">
         <v>0.84440231805742705</v>
       </c>
-      <c r="AB12" s="76">
+      <c r="AB12" s="37">
         <v>0.79784209579878396</v>
       </c>
       <c r="AC12" s="3">
         <v>0.782602473376379</v>
       </c>
-      <c r="AN12" s="74">
+      <c r="AN12" s="1">
         <v>0.67782924072056805</v>
       </c>
-      <c r="AO12" s="74">
+      <c r="AO12" s="1">
         <v>0.76128317671768697</v>
       </c>
-      <c r="AP12" s="76">
+      <c r="AP12" s="37">
         <v>0.70948968952475799</v>
       </c>
-      <c r="AQ12" s="74">
+      <c r="AQ12" s="1">
         <v>0.79507120946929399</v>
       </c>
-      <c r="AR12" s="2"/>
-      <c r="BB12" s="74">
+      <c r="BB12" s="1">
         <v>0.64726207355885201</v>
       </c>
-      <c r="BC12" s="74">
+      <c r="BC12" s="1">
         <v>0.71392502180581197</v>
       </c>
-      <c r="BD12" s="76">
+      <c r="BD12" s="37">
         <v>0.66269869294451</v>
       </c>
-      <c r="BE12" s="74">
+      <c r="BE12" s="1">
         <v>0.67089046763825799</v>
       </c>
-      <c r="BF12" s="2"/>
-      <c r="BP12" s="78">
+      <c r="BP12" s="6">
         <v>0.63143886434585295</v>
       </c>
-      <c r="BQ12" s="74">
+      <c r="BQ12" s="1">
         <v>0.62358771893880305</v>
       </c>
-      <c r="BR12" s="76">
+      <c r="BR12" s="37">
         <v>0.60773590056835503</v>
       </c>
       <c r="BS12" s="3">
         <v>0.66679034198289</v>
       </c>
-      <c r="BT12" s="74">
+      <c r="BT12" s="1">
         <f>N12/$J$4</f>
         <v>0.99112351119096165</v>
       </c>
-      <c r="BU12" s="74">
+      <c r="BU12" s="1">
         <f>AB12/$X$4</f>
         <v>0.96356427017180102</v>
       </c>
-      <c r="BV12" s="74">
+      <c r="BV12" s="1">
         <f>AP12/$AL$4</f>
         <v>0.87790287228953634</v>
       </c>
-      <c r="BW12" s="74">
+      <c r="BW12" s="1">
         <f>BD12/$AZ$4</f>
         <v>0.8200358862065299</v>
       </c>
-      <c r="BX12" s="74">
+      <c r="BX12" s="1">
         <f>BR12/$BN$4</f>
         <v>0.78196964806952485</v>
       </c>
-      <c r="BY12" s="79" t="s">
+      <c r="BY12" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="13" spans="1:77" x14ac:dyDescent="0.45">
-      <c r="A13" s="57"/>
+      <c r="A13" s="73"/>
       <c r="L13" s="1">
         <v>0.81018794972422004</v>
       </c>
@@ -11876,7 +11904,6 @@
       <c r="AC13" s="3">
         <v>0.78274129591092401</v>
       </c>
-      <c r="AD13" s="1"/>
       <c r="AN13" s="1">
         <v>0.69485587553230499</v>
       </c>
@@ -11901,13 +11928,13 @@
       <c r="BE13" s="1">
         <v>0.67468235768528095</v>
       </c>
-      <c r="BP13" s="78">
+      <c r="BP13" s="6">
         <v>0.628140843762788</v>
       </c>
-      <c r="BQ13" s="74">
+      <c r="BQ13" s="1">
         <v>0.61708429205579496</v>
       </c>
-      <c r="BR13" s="76">
+      <c r="BR13" s="37">
         <v>0.60475999359911503</v>
       </c>
       <c r="BS13" s="3">
@@ -11934,66 +11961,63 @@
         <v>0.7781405688210421</v>
       </c>
     </row>
-    <row r="14" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="67"/>
-      <c r="B14" s="2"/>
-      <c r="L14" s="74">
+    <row r="14" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A14" s="83"/>
+      <c r="L14" s="1">
         <v>0.811287308243271</v>
       </c>
-      <c r="M14" s="74">
+      <c r="M14" s="1">
         <v>0.88881786840493204</v>
       </c>
-      <c r="N14" s="76">
+      <c r="N14" s="37">
         <v>0.844937149186197</v>
       </c>
       <c r="O14" s="3">
         <v>0.78473633156113098</v>
       </c>
-      <c r="Z14" s="74">
+      <c r="Z14" s="1">
         <v>0.76220505232254498</v>
       </c>
-      <c r="AA14" s="74">
+      <c r="AA14" s="1">
         <v>0.84341837644633899</v>
       </c>
-      <c r="AB14" s="76">
+      <c r="AB14" s="37">
         <v>0.79653077143948803</v>
       </c>
       <c r="AC14" s="3">
         <v>0.78297356263177997</v>
       </c>
-      <c r="AN14" s="74">
+      <c r="AN14" s="1">
         <v>0.66642436972638297</v>
       </c>
-      <c r="AO14" s="74">
+      <c r="AO14" s="1">
         <v>0.74681042592740798</v>
       </c>
-      <c r="AP14" s="76">
+      <c r="AP14" s="37">
         <v>0.69721315342052004</v>
       </c>
-      <c r="AQ14" s="74">
+      <c r="AQ14" s="1">
         <v>0.79501960364755897</v>
       </c>
-      <c r="AR14" s="2"/>
-      <c r="BB14" s="74">
+      <c r="BB14" s="1">
         <v>0.67079257549225102</v>
       </c>
-      <c r="BC14" s="74">
+      <c r="BC14" s="1">
         <v>0.74026503412897404</v>
       </c>
-      <c r="BD14" s="76">
+      <c r="BD14" s="37">
         <v>0.68795520452583503</v>
       </c>
-      <c r="BE14" s="74">
+      <c r="BE14" s="1">
         <v>0.67085477824687001</v>
       </c>
-      <c r="BF14" s="2"/>
-      <c r="BP14" s="78">
+      <c r="BP14" s="6">
         <v>0.62166400223265905</v>
       </c>
-      <c r="BQ14" s="74">
+      <c r="BQ14" s="1">
         <v>0.61779315673134505</v>
       </c>
-      <c r="BR14" s="76">
+      <c r="BR14" s="37">
         <v>0.600366282527794</v>
       </c>
       <c r="BS14" s="3">
@@ -12019,10 +12043,9 @@
         <f>BR14/$BN$4</f>
         <v>0.77248721068151638</v>
       </c>
-      <c r="BY14" s="79"/>
     </row>
     <row r="15" spans="1:77" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="62" t="s">
+      <c r="A15" s="69" t="s">
         <v>116</v>
       </c>
       <c r="B15" s="17"/>
@@ -12108,186 +12131,178 @@
         <f>BR15/$BN$4</f>
         <v>0.73419441411334041</v>
       </c>
-      <c r="BY15" s="71" t="s">
+      <c r="BY15" s="45" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="16" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="57"/>
-      <c r="B16" s="2"/>
-      <c r="L16" s="74">
+    <row r="16" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A16" s="73"/>
+      <c r="L16" s="1">
         <v>0.76772042855283795</v>
       </c>
-      <c r="M16" s="74">
+      <c r="M16" s="1">
         <v>0.83951392909986799</v>
       </c>
-      <c r="N16" s="76">
+      <c r="N16" s="37">
         <v>0.796758536792332</v>
       </c>
       <c r="O16" s="3">
         <v>0.78546500597785995</v>
       </c>
-      <c r="Z16" s="74">
+      <c r="Z16" s="1">
         <v>0.66827064878702302</v>
       </c>
-      <c r="AA16" s="74">
+      <c r="AA16" s="1">
         <v>0.73515763936257705</v>
       </c>
-      <c r="AB16" s="76">
+      <c r="AB16" s="37">
         <v>0.693165824845142</v>
       </c>
       <c r="AC16" s="3">
         <v>0.78392771032184605</v>
       </c>
-      <c r="AN16" s="74">
+      <c r="AN16" s="1">
         <v>0.550794676070268</v>
       </c>
-      <c r="AO16" s="74">
+      <c r="AO16" s="1">
         <v>0.62379416105588503</v>
       </c>
-      <c r="AP16" s="76">
+      <c r="AP16" s="37">
         <v>0.57958306823762495</v>
       </c>
-      <c r="AQ16" s="74">
+      <c r="AQ16" s="1">
         <v>0.79685623797504901</v>
       </c>
-      <c r="AR16" s="2"/>
-      <c r="BB16" s="74">
+      <c r="BB16" s="1">
         <v>0.62456894099610105</v>
       </c>
-      <c r="BC16" s="74">
+      <c r="BC16" s="1">
         <v>0.68691627396864996</v>
       </c>
-      <c r="BD16" s="76">
+      <c r="BD16" s="37">
         <v>0.63825075388556696</v>
       </c>
-      <c r="BE16" s="74">
+      <c r="BE16" s="1">
         <v>0.66959116348542502</v>
       </c>
-      <c r="BF16" s="2"/>
-      <c r="BP16" s="78">
+      <c r="BP16" s="6">
         <v>0.58653004621336502</v>
       </c>
-      <c r="BQ16" s="74">
+      <c r="BQ16" s="1">
         <v>0.58344083632576704</v>
       </c>
-      <c r="BR16" s="76">
+      <c r="BR16" s="37">
         <v>0.56791131273690398</v>
       </c>
       <c r="BS16" s="3">
         <v>0.66815036026343599</v>
       </c>
-      <c r="BT16" s="74">
+      <c r="BT16" s="1">
         <f t="shared" ref="BT16:BT18" si="16">N16/$J$4</f>
         <v>0.93272192376298968</v>
       </c>
-      <c r="BU16" s="74">
+      <c r="BU16" s="1">
         <f t="shared" ref="BU16:BU18" si="17">AB16/$X$4</f>
         <v>0.83714537706392322</v>
       </c>
-      <c r="BV16" s="74">
+      <c r="BV16" s="1">
         <f t="shared" ref="BV16:BV18" si="18">AP16/$AL$4</f>
         <v>0.71716002057340367</v>
       </c>
-      <c r="BW16" s="74">
+      <c r="BW16" s="1">
         <f t="shared" ref="BW16:BW18" si="19">BD16/$AZ$4</f>
         <v>0.78978354440237564</v>
       </c>
-      <c r="BX16" s="74">
+      <c r="BX16" s="1">
         <f t="shared" ref="BX16:BX18" si="20">BR16/$BN$4</f>
         <v>0.73072762188356144</v>
       </c>
-      <c r="BY16" s="79"/>
     </row>
-    <row r="17" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="57"/>
-      <c r="B17" s="2"/>
-      <c r="L17" s="74">
+    <row r="17" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A17" s="73"/>
+      <c r="L17" s="1">
         <v>0.76270169122557596</v>
       </c>
-      <c r="M17" s="74">
+      <c r="M17" s="1">
         <v>0.83717472029125695</v>
       </c>
-      <c r="N17" s="76">
+      <c r="N17" s="37">
         <v>0.79436567904203803</v>
       </c>
       <c r="O17" s="3">
         <v>0.78545908404096998</v>
       </c>
-      <c r="Z17" s="74">
+      <c r="Z17" s="1">
         <v>0.67335271587507595</v>
       </c>
-      <c r="AA17" s="74">
+      <c r="AA17" s="1">
         <v>0.75030408430853102</v>
       </c>
-      <c r="AB17" s="76">
+      <c r="AB17" s="37">
         <v>0.70355199239269095</v>
       </c>
       <c r="AC17" s="3">
         <v>0.78493800563913996</v>
       </c>
-      <c r="AN17" s="74">
+      <c r="AN17" s="1">
         <v>0.55551263493412895</v>
       </c>
-      <c r="AO17" s="74">
+      <c r="AO17" s="1">
         <v>0.63452688894683895</v>
       </c>
-      <c r="AP17" s="76">
+      <c r="AP17" s="37">
         <v>0.58387868238307306</v>
       </c>
-      <c r="AQ17" s="74">
+      <c r="AQ17" s="1">
         <v>0.79418416299293804</v>
       </c>
-      <c r="AR17" s="2"/>
-      <c r="BB17" s="74">
+      <c r="BB17" s="1">
         <v>0.65496179888238804</v>
       </c>
-      <c r="BC17" s="74">
+      <c r="BC17" s="1">
         <v>0.72044587336750199</v>
       </c>
-      <c r="BD17" s="76">
+      <c r="BD17" s="37">
         <v>0.67053477715536103</v>
       </c>
-      <c r="BE17" s="74">
+      <c r="BE17" s="1">
         <v>0.67424911998273596</v>
       </c>
-      <c r="BF17" s="2"/>
-      <c r="BP17" s="78">
+      <c r="BP17" s="6">
         <v>0.58890006423427799</v>
       </c>
-      <c r="BQ17" s="74">
+      <c r="BQ17" s="1">
         <v>0.588162803735928</v>
       </c>
-      <c r="BR17" s="76">
+      <c r="BR17" s="37">
         <v>0.571101207008755</v>
       </c>
       <c r="BS17" s="3">
         <v>0.667264416864218</v>
       </c>
-      <c r="BT17" s="74">
+      <c r="BT17" s="1">
         <f t="shared" ref="BT17" si="21">N17/$J$4</f>
         <v>0.92992073522081142</v>
       </c>
-      <c r="BU17" s="74">
+      <c r="BU17" s="1">
         <f t="shared" ref="BU17" si="22">AB17/$X$4</f>
         <v>0.84968888661992936</v>
       </c>
-      <c r="BV17" s="74">
+      <c r="BV17" s="1">
         <f t="shared" ref="BV17" si="23">AP17/$AL$4</f>
         <v>0.72247529442757696</v>
       </c>
-      <c r="BW17" s="74">
+      <c r="BW17" s="1">
         <f t="shared" ref="BW17" si="24">BD17/$AZ$4</f>
         <v>0.8297324048939031</v>
       </c>
-      <c r="BX17" s="74">
+      <c r="BX17" s="1">
         <f t="shared" ref="BX17" si="25">BR17/$BN$4</f>
         <v>0.73483203713828904</v>
       </c>
-      <c r="BY17" s="79"/>
     </row>
     <row r="18" spans="1:77" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="67"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="26"/>
       <c r="L18" s="24">
         <v>0.75882164392513496</v>
@@ -12371,70 +12386,67 @@
         <f t="shared" si="20"/>
         <v>0.75490949525982043</v>
       </c>
-      <c r="BY18" s="72"/>
+      <c r="BY18" s="46"/>
     </row>
-    <row r="19" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="62" t="s">
+    <row r="19" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A19" s="69" t="s">
         <v>117</v>
       </c>
-      <c r="B19" s="2"/>
-      <c r="L19" s="74">
+      <c r="L19" s="1">
         <v>0.71338892634080198</v>
       </c>
-      <c r="M19" s="74">
+      <c r="M19" s="1">
         <v>0.78743784206086198</v>
       </c>
-      <c r="N19" s="76">
+      <c r="N19" s="37">
         <v>0.74492350051274003</v>
       </c>
       <c r="O19" s="3">
         <v>0.79731008533911896</v>
       </c>
-      <c r="Z19" s="74">
+      <c r="Z19" s="1">
         <v>0.61863884760952204</v>
       </c>
-      <c r="AA19" s="74">
+      <c r="AA19" s="1">
         <v>0.68419330569103398</v>
       </c>
-      <c r="AB19" s="76">
+      <c r="AB19" s="37">
         <v>0.64567819289774697</v>
       </c>
       <c r="AC19" s="3">
         <v>0.79961417650434796</v>
       </c>
-      <c r="AN19" s="74">
+      <c r="AN19" s="1">
         <v>0.55565087774468203</v>
       </c>
-      <c r="AO19" s="74">
+      <c r="AO19" s="1">
         <v>0.60395706946948402</v>
       </c>
-      <c r="AP19" s="76">
+      <c r="AP19" s="37">
         <v>0.57326385612122799</v>
       </c>
-      <c r="AQ19" s="74">
+      <c r="AQ19" s="1">
         <v>0.81217631187267703</v>
       </c>
-      <c r="AR19" s="2"/>
-      <c r="BB19" s="74">
+      <c r="BB19" s="1">
         <v>0.55954003654380002</v>
       </c>
-      <c r="BC19" s="74">
+      <c r="BC19" s="1">
         <v>0.59102916577935305</v>
       </c>
-      <c r="BD19" s="76">
+      <c r="BD19" s="37">
         <v>0.55119549494239195</v>
       </c>
-      <c r="BE19" s="74">
+      <c r="BE19" s="1">
         <v>0.68535661579045803</v>
       </c>
-      <c r="BF19" s="2"/>
-      <c r="BP19" s="78">
+      <c r="BP19" s="6">
         <v>0.51995296893758502</v>
       </c>
-      <c r="BQ19" s="74">
+      <c r="BQ19" s="1">
         <v>0.48936586628776502</v>
       </c>
-      <c r="BR19" s="76">
+      <c r="BR19" s="37">
         <v>0.49273792252989501</v>
       </c>
       <c r="BS19" s="3">
@@ -12460,10 +12472,9 @@
         <f t="shared" ref="BX19:BX24" si="30">BR19/$BN$4</f>
         <v>0.63400253220333413</v>
       </c>
-      <c r="BY19" s="79"/>
     </row>
     <row r="20" spans="1:77" x14ac:dyDescent="0.45">
-      <c r="A20" s="57"/>
+      <c r="A20" s="73"/>
       <c r="L20" s="1">
         <v>0.73026235202853895</v>
       </c>
@@ -12512,13 +12523,13 @@
       <c r="BE20" s="1">
         <v>0.68767623733433403</v>
       </c>
-      <c r="BP20" s="78">
+      <c r="BP20" s="6">
         <v>0.50273964589023001</v>
       </c>
-      <c r="BQ20" s="74">
+      <c r="BQ20" s="1">
         <v>0.47955433529526098</v>
       </c>
-      <c r="BR20" s="76">
+      <c r="BR20" s="37">
         <v>0.47559585347433903</v>
       </c>
       <c r="BS20" s="3">
@@ -12545,66 +12556,63 @@
         <v>0.61194594858860829</v>
       </c>
     </row>
-    <row r="21" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A21" s="67"/>
-      <c r="B21" s="2"/>
-      <c r="L21" s="74">
+    <row r="21" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A21" s="83"/>
+      <c r="L21" s="1">
         <v>0.731828088099445</v>
       </c>
-      <c r="M21" s="74">
+      <c r="M21" s="1">
         <v>0.80823855242762099</v>
       </c>
-      <c r="N21" s="76">
+      <c r="N21" s="37">
         <v>0.76457225153061803</v>
       </c>
       <c r="O21" s="3">
         <v>0.79763773181437303</v>
       </c>
-      <c r="Z21" s="74">
+      <c r="Z21" s="1">
         <v>0.65470965975614503</v>
       </c>
-      <c r="AA21" s="74">
+      <c r="AA21" s="1">
         <v>0.72014595145119298</v>
       </c>
-      <c r="AB21" s="76">
+      <c r="AB21" s="37">
         <v>0.68065275441996498</v>
       </c>
       <c r="AC21" s="3">
         <v>0.80065343646984899</v>
       </c>
-      <c r="AN21" s="74">
+      <c r="AN21" s="1">
         <v>0.52996294143755995</v>
       </c>
-      <c r="AO21" s="74">
+      <c r="AO21" s="1">
         <v>0.57537046208778098</v>
       </c>
-      <c r="AP21" s="76">
+      <c r="AP21" s="37">
         <v>0.545104230631132</v>
       </c>
-      <c r="AQ21" s="74">
+      <c r="AQ21" s="1">
         <v>0.81529525585184504</v>
       </c>
-      <c r="AR21" s="2"/>
-      <c r="BB21" s="74">
+      <c r="BB21" s="1">
         <v>0.57313281800180504</v>
       </c>
-      <c r="BC21" s="74">
+      <c r="BC21" s="1">
         <v>0.60367460175972698</v>
       </c>
-      <c r="BD21" s="76">
+      <c r="BD21" s="37">
         <v>0.56393118365922001</v>
       </c>
-      <c r="BE21" s="74">
+      <c r="BE21" s="1">
         <v>0.68815338213601696</v>
       </c>
-      <c r="BF21" s="2"/>
-      <c r="BP21" s="78">
+      <c r="BP21" s="6">
         <v>0.49135341493436901</v>
       </c>
-      <c r="BQ21" s="74">
+      <c r="BQ21" s="1">
         <v>0.46774532269626001</v>
       </c>
-      <c r="BR21" s="76">
+      <c r="BR21" s="37">
         <v>0.46397429463616802</v>
       </c>
       <c r="BS21" s="3">
@@ -12630,73 +12638,72 @@
         <f t="shared" si="30"/>
         <v>0.59699256790761679</v>
       </c>
-      <c r="BY21" s="79"/>
     </row>
-    <row r="22" spans="1:77" s="81" customFormat="1" ht="28" x14ac:dyDescent="0.45">
-      <c r="A22" s="82" t="s">
+    <row r="22" spans="1:77" s="48" customFormat="1" ht="28" x14ac:dyDescent="0.45">
+      <c r="A22" s="49" t="s">
         <v>113</v>
       </c>
-      <c r="B22" s="83"/>
-      <c r="L22" s="81">
+      <c r="B22" s="50"/>
+      <c r="L22" s="48">
         <v>0.81089707273063505</v>
       </c>
-      <c r="M22" s="81">
+      <c r="M22" s="48">
         <v>0.88633662736617203</v>
       </c>
-      <c r="N22" s="84">
+      <c r="N22" s="51">
         <v>0.84376761890553897</v>
       </c>
-      <c r="O22" s="85">
+      <c r="O22" s="52">
         <v>0.78460163549457396</v>
       </c>
-      <c r="Z22" s="81">
+      <c r="Z22" s="48">
         <v>0.765657939927325</v>
       </c>
-      <c r="AA22" s="81">
+      <c r="AA22" s="48">
         <v>0.84506484541962101</v>
       </c>
-      <c r="AB22" s="84">
+      <c r="AB22" s="51">
         <v>0.79932320317306405</v>
       </c>
-      <c r="AC22" s="85">
+      <c r="AC22" s="52">
         <v>0.78301534293072395</v>
       </c>
-      <c r="AN22" s="81">
+      <c r="AN22" s="48">
         <v>0.67609246532134504</v>
       </c>
-      <c r="AO22" s="81">
+      <c r="AO22" s="48">
         <v>0.76290947662860797</v>
       </c>
-      <c r="AP22" s="84">
+      <c r="AP22" s="51">
         <v>0.71247069010796804</v>
       </c>
-      <c r="AQ22" s="81">
+      <c r="AQ22" s="48">
         <v>0.79774847532711701</v>
       </c>
-      <c r="AR22" s="83"/>
-      <c r="BB22" s="81">
+      <c r="AR22" s="50"/>
+      <c r="BB22" s="48">
         <v>0.66313759304054498</v>
       </c>
-      <c r="BC22" s="81">
+      <c r="BC22" s="48">
         <v>0.72792814163387098</v>
       </c>
-      <c r="BD22" s="84">
+      <c r="BD22" s="51">
         <v>0.678062571182795</v>
       </c>
-      <c r="BE22" s="81">
+      <c r="BE22" s="48">
         <v>0.67118014237401802</v>
       </c>
-      <c r="BF22" s="83"/>
-      <c r="BP22" s="88">
+      <c r="BF22" s="50"/>
+      <c r="BP22" s="55">
         <v>0.63688602089269597</v>
       </c>
-      <c r="BQ22" s="81">
+      <c r="BQ22" s="48">
         <v>0.63022740847028202</v>
       </c>
-      <c r="BR22" s="84">
+      <c r="BR22" s="51">
         <v>0.61538217870323997</v>
       </c>
-      <c r="BS22" s="85">
+      <c r="BS22" s="52">
         <v>0.66521942940705503</v>
       </c>
       <c r="BT22" s="24">
@@ -12719,72 +12726,69 @@
         <f t="shared" si="30"/>
         <v>0.79180806211843313</v>
       </c>
-      <c r="BY22" s="86" t="s">
+      <c r="BY22" s="53" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="23" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A23" s="66" t="s">
+    <row r="23" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A23" s="82" t="s">
         <v>109</v>
       </c>
-      <c r="B23" s="2"/>
-      <c r="L23" s="74">
+      <c r="L23" s="1">
         <v>0.79757165713288602</v>
       </c>
-      <c r="M23" s="74">
+      <c r="M23" s="1">
         <v>0.872118813378715</v>
       </c>
-      <c r="N23" s="76">
+      <c r="N23" s="37">
         <v>0.82918907393234997</v>
       </c>
       <c r="O23" s="3">
         <v>0.78526984834650004</v>
       </c>
-      <c r="Z23" s="74">
+      <c r="Z23" s="1">
         <v>0.74205668228761401</v>
       </c>
-      <c r="AA23" s="74">
+      <c r="AA23" s="1">
         <v>0.81755265027334501</v>
       </c>
-      <c r="AB23" s="76">
+      <c r="AB23" s="37">
         <v>0.77182777220285703</v>
       </c>
       <c r="AC23" s="3">
         <v>0.78506582734152497</v>
       </c>
-      <c r="AN23" s="74">
+      <c r="AN23" s="1">
         <v>0.68919037194125299</v>
       </c>
-      <c r="AO23" s="74">
+      <c r="AO23" s="1">
         <v>0.76748648031195699</v>
       </c>
-      <c r="AP23" s="76">
+      <c r="AP23" s="37">
         <v>0.72026639954081095</v>
       </c>
-      <c r="AQ23" s="74">
+      <c r="AQ23" s="1">
         <v>0.79761151804462305</v>
       </c>
-      <c r="AR23" s="2"/>
-      <c r="BB23" s="74">
+      <c r="BB23" s="1">
         <v>0.62914124573501395</v>
       </c>
-      <c r="BC23" s="74">
+      <c r="BC23" s="1">
         <v>0.67959204719002198</v>
       </c>
-      <c r="BD23" s="76">
+      <c r="BD23" s="37">
         <v>0.63320267339030201</v>
       </c>
-      <c r="BE23" s="74">
+      <c r="BE23" s="1">
         <v>0.67384863218630497</v>
       </c>
-      <c r="BF23" s="2"/>
-      <c r="BP23" s="78">
+      <c r="BP23" s="6">
         <v>0.59412958100360702</v>
       </c>
-      <c r="BQ23" s="74">
+      <c r="BQ23" s="1">
         <v>0.58280258686233599</v>
       </c>
-      <c r="BR23" s="76">
+      <c r="BR23" s="37">
         <v>0.56886063403504605</v>
       </c>
       <c r="BS23" s="3">
@@ -12810,10 +12814,9 @@
         <f t="shared" si="30"/>
         <v>0.73194910713845396</v>
       </c>
-      <c r="BY23" s="79"/>
     </row>
     <row r="24" spans="1:77" x14ac:dyDescent="0.45">
-      <c r="A24" s="57"/>
+      <c r="A24" s="73"/>
       <c r="L24" s="1">
         <v>0.79631487330023598</v>
       </c>
@@ -12862,13 +12865,13 @@
       <c r="BE24" s="1">
         <v>0.67416020382716402</v>
       </c>
-      <c r="BP24" s="78">
+      <c r="BP24" s="6">
         <v>0.60005500599981298</v>
       </c>
-      <c r="BQ24" s="74">
+      <c r="BQ24" s="1">
         <v>0.59419276534731702</v>
       </c>
-      <c r="BR24" s="76">
+      <c r="BR24" s="37">
         <v>0.58130433666571402</v>
       </c>
       <c r="BS24" s="3">
@@ -12895,95 +12898,91 @@
         <v>0.74796033464317302</v>
       </c>
     </row>
-    <row r="25" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="67"/>
-      <c r="B25" s="2"/>
-      <c r="L25" s="74">
+    <row r="25" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A25" s="83"/>
+      <c r="L25" s="1">
         <v>0.79659213585573896</v>
       </c>
-      <c r="M25" s="74">
+      <c r="M25" s="1">
         <v>0.871157359954287</v>
       </c>
-      <c r="N25" s="76">
+      <c r="N25" s="37">
         <v>0.82818156897616102</v>
       </c>
       <c r="O25" s="3">
         <v>0.78551469705243704</v>
       </c>
-      <c r="Z25" s="74">
+      <c r="Z25" s="1">
         <v>0.73844967364008396</v>
       </c>
-      <c r="AA25" s="74">
+      <c r="AA25" s="1">
         <v>0.81289495557423197</v>
       </c>
-      <c r="AB25" s="76">
+      <c r="AB25" s="37">
         <v>0.76783775574373603</v>
       </c>
       <c r="AC25" s="3">
         <v>0.78467311992053301</v>
       </c>
-      <c r="AN25" s="74">
+      <c r="AN25" s="1">
         <v>0.69624413024181997</v>
       </c>
-      <c r="AO25" s="74">
+      <c r="AO25" s="1">
         <v>0.77266785998239795</v>
       </c>
-      <c r="AP25" s="76">
+      <c r="AP25" s="37">
         <v>0.72566557748558402</v>
       </c>
-      <c r="AQ25" s="74">
+      <c r="AQ25" s="1">
         <v>0.79788286323660296</v>
       </c>
-      <c r="AR25" s="2"/>
-      <c r="BB25" s="74">
+      <c r="BB25" s="1">
         <v>0.65178128763308696</v>
       </c>
-      <c r="BC25" s="74">
+      <c r="BC25" s="1">
         <v>0.71035381778656304</v>
       </c>
-      <c r="BD25" s="76">
+      <c r="BD25" s="37">
         <v>0.66715458249196802</v>
       </c>
-      <c r="BE25" s="74">
+      <c r="BE25" s="1">
         <v>0.67349925627019902</v>
       </c>
-      <c r="BF25" s="2"/>
-      <c r="BP25" s="78">
+      <c r="BP25" s="6">
         <v>0.59589735729410198</v>
       </c>
-      <c r="BQ25" s="74">
+      <c r="BQ25" s="1">
         <v>0.58772249013065203</v>
       </c>
-      <c r="BR25" s="76">
+      <c r="BR25" s="37">
         <v>0.57567752344846901</v>
       </c>
       <c r="BS25" s="3">
         <v>0.66622575593539302</v>
       </c>
-      <c r="BT25" s="74">
+      <c r="BT25" s="1">
         <f>N25/$J$4</f>
         <v>0.96950716003665693</v>
       </c>
-      <c r="BU25" s="74">
+      <c r="BU25" s="1">
         <f>AB25/$X$4</f>
         <v>0.9273276386636784</v>
       </c>
-      <c r="BV25" s="74">
+      <c r="BV25" s="1">
         <f t="shared" ref="BV25" si="31">AP25/$AL$4</f>
         <v>0.89791846760023797</v>
       </c>
-      <c r="BW25" s="74">
+      <c r="BW25" s="1">
         <f>BD25/$AZ$4</f>
         <v>0.82554968813912877</v>
       </c>
-      <c r="BX25" s="74">
+      <c r="BX25" s="1">
         <f>BR25/$BN$4</f>
         <v>0.74072035236283196</v>
       </c>
-      <c r="BY25" s="79"/>
     </row>
     <row r="26" spans="1:77" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="82" t="s">
         <v>114</v>
       </c>
       <c r="B26" s="17"/>
@@ -13049,117 +13048,113 @@
       <c r="BS26" s="20">
         <v>0.66694824888583104</v>
       </c>
-      <c r="BT26" s="74">
+      <c r="BT26" s="1">
         <f t="shared" ref="BT26:BT28" si="32">N26/$J$4</f>
         <v>0.98854315977377705</v>
       </c>
-      <c r="BU26" s="74">
+      <c r="BU26" s="1">
         <f t="shared" ref="BU26:BU28" si="33">AB26/$X$4</f>
         <v>0.95864881480438469</v>
       </c>
-      <c r="BV26" s="74">
+      <c r="BV26" s="1">
         <f t="shared" ref="BV26:BV28" si="34">AP26/$AL$4</f>
         <v>0.87453097137342573</v>
       </c>
-      <c r="BW26" s="74">
+      <c r="BW26" s="1">
         <f t="shared" ref="BW26:BW28" si="35">BD26/$AZ$4</f>
         <v>0.8474786464023869</v>
       </c>
-      <c r="BX26" s="74">
+      <c r="BX26" s="1">
         <f t="shared" ref="BX26:BX28" si="36">BR26/$BN$4</f>
         <v>0.77410267414960732</v>
       </c>
-      <c r="BY26" s="71"/>
+      <c r="BY26" s="45"/>
     </row>
-    <row r="27" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="57"/>
-      <c r="B27" s="2"/>
-      <c r="L27" s="74">
+    <row r="27" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A27" s="73"/>
+      <c r="L27" s="1">
         <v>0.80328936067702394</v>
       </c>
-      <c r="M27" s="74">
+      <c r="M27" s="1">
         <v>0.88931478863746205</v>
       </c>
-      <c r="N27" s="76">
+      <c r="N27" s="37">
         <v>0.83947667938304305</v>
       </c>
       <c r="O27" s="3">
         <v>0.78422776556089802</v>
       </c>
-      <c r="Z27" s="74">
+      <c r="Z27" s="1">
         <v>0.74618614657966298</v>
       </c>
-      <c r="AA27" s="74">
+      <c r="AA27" s="1">
         <v>0.83756286325439</v>
       </c>
-      <c r="AB27" s="76">
+      <c r="AB27" s="37">
         <v>0.785239190463908</v>
       </c>
       <c r="AC27" s="3">
         <v>0.78137083802072405</v>
       </c>
-      <c r="AN27" s="74">
+      <c r="AN27" s="1">
         <v>0.64765309658574499</v>
       </c>
-      <c r="AO27" s="74">
+      <c r="AO27" s="1">
         <v>0.72510956812043403</v>
       </c>
-      <c r="AP27" s="76">
+      <c r="AP27" s="37">
         <v>0.678089751887056</v>
       </c>
-      <c r="AQ27" s="74">
+      <c r="AQ27" s="1">
         <v>0.77719747082568003</v>
       </c>
-      <c r="AR27" s="2"/>
-      <c r="BB27" s="74">
+      <c r="BB27" s="1">
         <v>0.66597397735882402</v>
       </c>
-      <c r="BC27" s="74">
+      <c r="BC27" s="1">
         <v>0.72522647304287702</v>
       </c>
-      <c r="BD27" s="76">
+      <c r="BD27" s="37">
         <v>0.67874152091892304</v>
       </c>
-      <c r="BE27" s="74">
+      <c r="BE27" s="1">
         <v>0.66730840424135895</v>
       </c>
-      <c r="BF27" s="2"/>
-      <c r="BP27" s="78">
+      <c r="BP27" s="6">
         <v>0.62215284176307695</v>
       </c>
-      <c r="BQ27" s="74">
+      <c r="BQ27" s="1">
         <v>0.62307657800909899</v>
       </c>
-      <c r="BR27" s="76">
+      <c r="BR27" s="37">
         <v>0.60253357256996398</v>
       </c>
       <c r="BS27" s="3">
         <v>0.66147152849227997</v>
       </c>
-      <c r="BT27" s="74">
+      <c r="BT27" s="1">
         <f t="shared" si="32"/>
         <v>0.98272973202218716</v>
       </c>
-      <c r="BU27" s="74">
+      <c r="BU27" s="1">
         <f t="shared" si="33"/>
         <v>0.94834357757487053</v>
       </c>
-      <c r="BV27" s="74">
+      <c r="BV27" s="1">
         <f t="shared" si="34"/>
         <v>0.83904945997241631</v>
       </c>
-      <c r="BW27" s="74">
+      <c r="BW27" s="1">
         <f t="shared" si="35"/>
         <v>0.8398875847164563</v>
       </c>
-      <c r="BX27" s="74">
+      <c r="BX27" s="1">
         <f t="shared" si="36"/>
         <v>0.77527584803197624</v>
       </c>
-      <c r="BY27" s="79"/>
     </row>
     <row r="28" spans="1:77" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="67"/>
+      <c r="A28" s="83"/>
       <c r="B28" s="26"/>
       <c r="L28" s="24">
         <v>0.81244761722029402</v>
@@ -13223,30 +13218,30 @@
       <c r="BS28" s="25">
         <v>0.66576874557126098</v>
       </c>
-      <c r="BT28" s="74">
+      <c r="BT28" s="1">
         <f t="shared" si="32"/>
         <v>0.98877818695407604</v>
       </c>
-      <c r="BU28" s="74">
+      <c r="BU28" s="1">
         <f t="shared" si="33"/>
         <v>0.95985968720219395</v>
       </c>
-      <c r="BV28" s="74">
+      <c r="BV28" s="1">
         <f t="shared" si="34"/>
         <v>0.88977698903975622</v>
       </c>
-      <c r="BW28" s="74">
+      <c r="BW28" s="1">
         <f t="shared" si="35"/>
         <v>0.82915772286485234</v>
       </c>
-      <c r="BX28" s="74">
+      <c r="BX28" s="1">
         <f t="shared" si="36"/>
         <v>0.76975106365367019</v>
       </c>
-      <c r="BY28" s="72"/>
+      <c r="BY28" s="46"/>
     </row>
     <row r="29" spans="1:77" s="16" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="82" t="s">
         <v>130</v>
       </c>
       <c r="B29" s="17">
@@ -13479,131 +13474,131 @@
         <f>BR29/BN29</f>
         <v>0.73890900811177462</v>
       </c>
-      <c r="BY29" s="71"/>
+      <c r="BY29" s="45"/>
     </row>
-    <row r="30" spans="1:77" s="74" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A30" s="57"/>
+    <row r="30" spans="1:77" x14ac:dyDescent="0.45">
+      <c r="A30" s="73"/>
       <c r="B30" s="2">
         <v>0.40058309037900802</v>
       </c>
-      <c r="C30" s="74">
+      <c r="C30" s="1">
         <v>0.76964022726456205</v>
       </c>
-      <c r="D30" s="74">
+      <c r="D30" s="1">
         <v>0.90236233025327395</v>
       </c>
-      <c r="E30" s="74">
+      <c r="E30" s="1">
         <v>0.83996506829016604</v>
       </c>
-      <c r="F30" s="74">
+      <c r="F30" s="1">
         <v>0.86901157570623999</v>
       </c>
-      <c r="G30" s="74">
+      <c r="G30" s="1">
         <v>0.58571428571428497</v>
       </c>
-      <c r="H30" s="74">
+      <c r="H30" s="1">
         <v>0.80006393946348597</v>
       </c>
-      <c r="I30" s="74">
+      <c r="I30" s="1">
         <v>0.88825249045000698</v>
       </c>
-      <c r="J30" s="74">
+      <c r="J30" s="1">
         <v>0.84070673971183796</v>
       </c>
-      <c r="K30" s="74">
+      <c r="K30" s="1">
         <v>0.77726649712517704</v>
       </c>
-      <c r="L30" s="74">
+      <c r="L30" s="1">
         <v>0.79415679991741905</v>
       </c>
-      <c r="M30" s="74">
+      <c r="M30" s="1">
         <v>0.87585717084251502</v>
       </c>
-      <c r="N30" s="76">
+      <c r="N30" s="37">
         <v>0.82956706879386399</v>
       </c>
       <c r="O30" s="3">
         <v>0.78068984153702903</v>
       </c>
-      <c r="P30" s="74">
+      <c r="P30" s="1">
         <v>0.33205608774121897</v>
       </c>
-      <c r="Q30" s="74">
+      <c r="Q30" s="1">
         <v>0.75243633730197801</v>
       </c>
-      <c r="R30" s="74">
+      <c r="R30" s="1">
         <v>0.87215625665658503</v>
       </c>
-      <c r="S30" s="74">
+      <c r="S30" s="1">
         <v>0.84558445284568395</v>
       </c>
-      <c r="T30" s="74">
+      <c r="T30" s="1">
         <v>0.85786447680767497</v>
       </c>
-      <c r="U30" s="74">
+      <c r="U30" s="1">
         <v>0.53565181174510601</v>
       </c>
-      <c r="V30" s="74">
+      <c r="V30" s="1">
         <v>0.7679938294259</v>
       </c>
-      <c r="W30" s="74">
+      <c r="W30" s="1">
         <v>0.87452969811514003</v>
       </c>
-      <c r="X30" s="74">
+      <c r="X30" s="1">
         <v>0.81690701533298105</v>
       </c>
-      <c r="Y30" s="74">
+      <c r="Y30" s="1">
         <v>0.78225247280618104</v>
       </c>
-      <c r="Z30" s="74">
+      <c r="Z30" s="1">
         <v>0.75193405571863303</v>
       </c>
-      <c r="AA30" s="74">
+      <c r="AA30" s="1">
         <v>0.842776920075053</v>
       </c>
-      <c r="AB30" s="76">
+      <c r="AB30" s="37">
         <v>0.79066418375341496</v>
       </c>
       <c r="AC30" s="3">
         <v>0.78792008100257105</v>
       </c>
-      <c r="AD30" s="74">
+      <c r="AD30" s="1">
         <v>0.27857142857142803</v>
       </c>
-      <c r="AE30" s="74">
+      <c r="AE30" s="1">
         <v>0.75789113322060897</v>
       </c>
-      <c r="AF30" s="74">
+      <c r="AF30" s="1">
         <v>0.867022591557296</v>
       </c>
-      <c r="AG30" s="74">
+      <c r="AG30" s="1">
         <v>0.85749807472531803</v>
       </c>
-      <c r="AH30" s="74">
+      <c r="AH30" s="1">
         <v>0.86182852336279403</v>
       </c>
-      <c r="AI30" s="74">
+      <c r="AI30" s="1">
         <v>0.44856309870887101</v>
       </c>
-      <c r="AJ30" s="74">
+      <c r="AJ30" s="1">
         <v>0.73118628259056095</v>
       </c>
-      <c r="AK30" s="74">
+      <c r="AK30" s="1">
         <v>0.86213655189228899</v>
       </c>
-      <c r="AL30" s="74">
+      <c r="AL30" s="1">
         <v>0.790813768498281</v>
       </c>
-      <c r="AM30" s="74">
+      <c r="AM30" s="1">
         <v>0.77758698966420603</v>
       </c>
-      <c r="AN30" s="74">
+      <c r="AN30" s="1">
         <v>0.68996910250659405</v>
       </c>
-      <c r="AO30" s="74">
+      <c r="AO30" s="1">
         <v>0.79922511081979297</v>
       </c>
-      <c r="AP30" s="76">
+      <c r="AP30" s="37">
         <v>0.73461861881370505</v>
       </c>
       <c r="AQ30" s="3">
@@ -13612,40 +13607,40 @@
       <c r="AR30" s="2">
         <v>0.29217687074829901</v>
       </c>
-      <c r="AS30" s="74">
+      <c r="AS30" s="1">
         <v>0.651528847667593</v>
       </c>
-      <c r="AT30" s="74">
+      <c r="AT30" s="1">
         <v>0.81234582879531103</v>
       </c>
-      <c r="AU30" s="74">
+      <c r="AU30" s="1">
         <v>0.77080131548545505</v>
       </c>
-      <c r="AV30" s="74">
+      <c r="AV30" s="1">
         <v>0.78593175808906302</v>
       </c>
-      <c r="AW30" s="74">
+      <c r="AW30" s="1">
         <v>0.39047619047618998</v>
       </c>
-      <c r="AX30" s="74">
+      <c r="AX30" s="1">
         <v>0.77509902619845095</v>
       </c>
-      <c r="AY30" s="74">
+      <c r="AY30" s="1">
         <v>0.83944974945684903</v>
       </c>
-      <c r="AZ30" s="74">
+      <c r="AZ30" s="1">
         <v>0.80133885960541396</v>
       </c>
-      <c r="BA30" s="74">
+      <c r="BA30" s="1">
         <v>0.65179013401555397</v>
       </c>
-      <c r="BB30" s="74">
+      <c r="BB30" s="1">
         <v>0.63294006365071698</v>
       </c>
-      <c r="BC30" s="74">
+      <c r="BC30" s="1">
         <v>0.71217252976059298</v>
       </c>
-      <c r="BD30" s="76">
+      <c r="BD30" s="37">
         <v>0.65246685216093703</v>
       </c>
       <c r="BE30" s="3">
@@ -13654,40 +13649,40 @@
       <c r="BF30" s="2">
         <v>0.24115646258503401</v>
       </c>
-      <c r="BG30" s="74">
+      <c r="BG30" s="1">
         <v>0.66883971691382904</v>
       </c>
-      <c r="BH30" s="74">
+      <c r="BH30" s="1">
         <v>0.81137792073111603</v>
       </c>
-      <c r="BI30" s="74">
+      <c r="BI30" s="1">
         <v>0.79284179548899003</v>
       </c>
-      <c r="BJ30" s="74">
+      <c r="BJ30" s="1">
         <v>0.79905215097382998</v>
       </c>
-      <c r="BK30" s="74">
+      <c r="BK30" s="1">
         <v>0.37414965986394499</v>
       </c>
-      <c r="BL30" s="74">
+      <c r="BL30" s="1">
         <v>0.74793840048917404</v>
       </c>
-      <c r="BM30" s="74">
+      <c r="BM30" s="1">
         <v>0.80834575302890099</v>
       </c>
-      <c r="BN30" s="74">
+      <c r="BN30" s="1">
         <v>0.77410235717153297</v>
       </c>
-      <c r="BO30" s="74">
+      <c r="BO30" s="1">
         <v>0.67035549337154299</v>
       </c>
-      <c r="BP30" s="78">
+      <c r="BP30" s="6">
         <v>0.55600406553341297</v>
       </c>
-      <c r="BQ30" s="74">
+      <c r="BQ30" s="1">
         <v>0.61644062378881004</v>
       </c>
-      <c r="BR30" s="76">
+      <c r="BR30" s="37">
         <v>0.56512566163604805</v>
       </c>
       <c r="BS30" s="3">
@@ -13713,10 +13708,9 @@
         <f>BR30/BN30</f>
         <v>0.73003997003825438</v>
       </c>
-      <c r="BY30" s="79"/>
     </row>
     <row r="31" spans="1:77" s="24" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A31" s="67"/>
+      <c r="A31" s="83"/>
       <c r="B31" s="26">
         <v>0.36143273635985002</v>
       </c>
@@ -13947,59 +13941,59 @@
         <f>BR31/BN31</f>
         <v>0.74970625319983231</v>
       </c>
-      <c r="BY31" s="72"/>
+      <c r="BY31" s="46"/>
     </row>
     <row r="36" spans="2:36" x14ac:dyDescent="0.45">
-      <c r="R36" s="44" t="s">
+      <c r="R36" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="S36" s="44"/>
-      <c r="T36" s="44"/>
-      <c r="U36" s="44"/>
-      <c r="V36" s="44"/>
-      <c r="W36" s="44"/>
-      <c r="X36" s="44"/>
-      <c r="Y36" s="44"/>
-      <c r="Z36" s="44"/>
-      <c r="AE36" s="44" t="s">
+      <c r="S36" s="64"/>
+      <c r="T36" s="64"/>
+      <c r="U36" s="64"/>
+      <c r="V36" s="64"/>
+      <c r="W36" s="64"/>
+      <c r="X36" s="64"/>
+      <c r="Y36" s="64"/>
+      <c r="Z36" s="64"/>
+      <c r="AE36" s="64" t="s">
         <v>140</v>
       </c>
-      <c r="AF36" s="44"/>
-      <c r="AG36" s="44"/>
-      <c r="AH36" s="44"/>
-      <c r="AI36" s="44"/>
-      <c r="AJ36" s="44"/>
+      <c r="AF36" s="64"/>
+      <c r="AG36" s="64"/>
+      <c r="AH36" s="64"/>
+      <c r="AI36" s="64"/>
+      <c r="AJ36" s="64"/>
     </row>
     <row r="37" spans="2:36" x14ac:dyDescent="0.45">
-      <c r="R37" s="44" t="s">
+      <c r="R37" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="S37" s="44"/>
-      <c r="T37" s="44"/>
-      <c r="U37" s="44" t="s">
+      <c r="S37" s="64"/>
+      <c r="T37" s="64"/>
+      <c r="U37" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="V37" s="44"/>
-      <c r="W37" s="44"/>
-      <c r="X37" s="44" t="s">
+      <c r="V37" s="64"/>
+      <c r="W37" s="64"/>
+      <c r="X37" s="64" t="s">
         <v>136</v>
       </c>
-      <c r="Y37" s="44"/>
-      <c r="Z37" s="44"/>
-      <c r="AA37" s="90"/>
-      <c r="AB37" s="90"/>
-      <c r="AC37" s="91"/>
-      <c r="AD37" s="92"/>
-      <c r="AE37" s="89" t="s">
+      <c r="Y37" s="64"/>
+      <c r="Z37" s="64"/>
+      <c r="AA37" s="56"/>
+      <c r="AB37" s="56"/>
+      <c r="AC37" s="57"/>
+      <c r="AD37" s="58"/>
+      <c r="AE37" s="64" t="s">
         <v>134</v>
       </c>
-      <c r="AF37" s="89"/>
-      <c r="AG37" s="89"/>
-      <c r="AH37" s="44" t="s">
+      <c r="AF37" s="64"/>
+      <c r="AG37" s="64"/>
+      <c r="AH37" s="64" t="s">
         <v>135</v>
       </c>
-      <c r="AI37" s="44"/>
-      <c r="AJ37" s="44"/>
+      <c r="AI37" s="64"/>
+      <c r="AJ37" s="64"/>
     </row>
     <row r="38" spans="2:36" x14ac:dyDescent="0.45">
       <c r="R38" s="1" t="s">
@@ -14030,7 +14024,6 @@
         <v>137</v>
       </c>
       <c r="AB38" s="1"/>
-      <c r="AD38" s="1"/>
       <c r="AE38" s="1" t="s">
         <v>132</v>
       </c>
@@ -14055,7 +14048,7 @@
         <v>131</v>
       </c>
       <c r="R39" s="1">
-        <f>$J$4</f>
+        <f t="shared" ref="R39:R44" si="37">$J$4</f>
         <v>0.854229450914883</v>
       </c>
       <c r="S39" s="1">
@@ -14063,11 +14056,11 @@
         <v>0.84445948275160387</v>
       </c>
       <c r="T39" s="1">
-        <f>S39/R39</f>
+        <f t="shared" ref="T39:T45" si="38">S39/R39</f>
         <v>0.98856282916397287</v>
       </c>
       <c r="U39" s="1">
-        <f>$X$4</f>
+        <f t="shared" ref="U39:U44" si="39">$X$4</f>
         <v>0.82801129151097597</v>
       </c>
       <c r="V39" s="1">
@@ -14075,11 +14068,11 @@
         <v>0.79887297652338618</v>
       </c>
       <c r="W39" s="1">
-        <f>V39/U39</f>
+        <f t="shared" ref="W39:W45" si="40">V39/U39</f>
         <v>0.96480927822322637</v>
       </c>
       <c r="X39" s="1">
-        <f>$AL$4</f>
+        <f t="shared" ref="X39:X44" si="41">$AL$4</f>
         <v>0.80816421943629901</v>
       </c>
       <c r="Y39" s="1">
@@ -14087,11 +14080,11 @@
         <v>0.73016410300189505</v>
       </c>
       <c r="Z39" s="1">
-        <f>Y39/X39</f>
+        <f t="shared" ref="Z39:Z45" si="42">Y39/X39</f>
         <v>0.90348481835930616</v>
       </c>
       <c r="AE39" s="1">
-        <f>$AZ$4</f>
+        <f t="shared" ref="AE39:AE44" si="43">$AZ$4</f>
         <v>0.80813377084037297</v>
       </c>
       <c r="AF39" s="1">
@@ -14099,11 +14092,11 @@
         <v>0.67550897682423194</v>
       </c>
       <c r="AG39" s="1">
-        <f>AF39/AE39</f>
+        <f t="shared" ref="AG39:AG45" si="44">AF39/AE39</f>
         <v>0.83588757356566679</v>
       </c>
       <c r="AH39" s="1">
-        <f>$BN$4</f>
+        <f t="shared" ref="AH39:AH44" si="45">$BN$4</f>
         <v>0.77718604816528802</v>
       </c>
       <c r="AI39" s="1">
@@ -14111,12 +14104,12 @@
         <v>0.60438812206283954</v>
       </c>
       <c r="AJ39" s="1">
-        <f>AI39/AH39</f>
+        <f t="shared" ref="AJ39:AJ45" si="46">AI39/AH39</f>
         <v>0.77766208424562622</v>
       </c>
     </row>
     <row r="40" spans="2:36" x14ac:dyDescent="0.45">
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="47" t="s">
         <v>118</v>
       </c>
       <c r="D40" s="14" t="s">
@@ -14126,7 +14119,7 @@
         <v>138</v>
       </c>
       <c r="R40" s="1">
-        <f>$J$4</f>
+        <f t="shared" si="37"/>
         <v>0.854229450914883</v>
       </c>
       <c r="S40" s="1">
@@ -14134,11 +14127,11 @@
         <v>0.84059909148824941</v>
       </c>
       <c r="T40" s="1">
-        <f>S40/R40</f>
+        <f t="shared" si="38"/>
         <v>0.98404367888272237</v>
       </c>
       <c r="U40" s="1">
-        <f>$X$4</f>
+        <f t="shared" si="39"/>
         <v>0.82801129151097597</v>
       </c>
       <c r="V40" s="1">
@@ -14146,11 +14139,11 @@
         <v>0.79342206902162937</v>
       </c>
       <c r="W40" s="1">
-        <f>V40/U40</f>
+        <f t="shared" si="40"/>
         <v>0.95822614637751224</v>
       </c>
       <c r="X40" s="1">
-        <f>$AL$4</f>
+        <f t="shared" si="41"/>
         <v>0.80816421943629901</v>
       </c>
       <c r="Y40" s="1">
@@ -14158,11 +14151,11 @@
         <v>0.71130702438280258</v>
       </c>
       <c r="Z40" s="1">
-        <f>Y40/X40</f>
+        <f t="shared" si="42"/>
         <v>0.8801515920600208</v>
       </c>
       <c r="AE40" s="1">
-        <f>$AZ$4</f>
+        <f t="shared" si="43"/>
         <v>0.80813377084037297</v>
       </c>
       <c r="AF40" s="1">
@@ -14170,11 +14163,11 @@
         <v>0.67033051749415273</v>
       </c>
       <c r="AG40" s="1">
-        <f>AF40/AE40</f>
+        <f t="shared" si="44"/>
         <v>0.82947965012906277</v>
       </c>
       <c r="AH40" s="1">
-        <f>$BN$4</f>
+        <f t="shared" si="45"/>
         <v>0.77718604816528802</v>
       </c>
       <c r="AI40" s="1">
@@ -14182,7 +14175,7 @@
         <v>0.60341353589550462</v>
       </c>
       <c r="AJ40" s="1">
-        <f>AI40/AH40</f>
+        <f t="shared" si="46"/>
         <v>0.77640809085545193</v>
       </c>
     </row>
@@ -14215,7 +14208,7 @@
         <v>141</v>
       </c>
       <c r="R41" s="1">
-        <f>$J$4</f>
+        <f t="shared" si="37"/>
         <v>0.854229450914883</v>
       </c>
       <c r="S41" s="1">
@@ -14223,11 +14216,11 @@
         <v>0.84285426922688467</v>
       </c>
       <c r="T41" s="1">
-        <f>S41/R41</f>
+        <f t="shared" si="38"/>
         <v>0.98668369291668012</v>
       </c>
       <c r="U41" s="1">
-        <f>$X$4</f>
+        <f t="shared" si="39"/>
         <v>0.82801129151097597</v>
       </c>
       <c r="V41" s="1">
@@ -14235,11 +14228,11 @@
         <v>0.79126196432838769</v>
       </c>
       <c r="W41" s="1">
-        <f>V41/U41</f>
+        <f t="shared" si="40"/>
         <v>0.95561735986048313</v>
       </c>
       <c r="X41" s="1">
-        <f>$AL$4</f>
+        <f t="shared" si="41"/>
         <v>0.80816421943629901</v>
       </c>
       <c r="Y41" s="1">
@@ -14247,11 +14240,11 @@
         <v>0.70131343918654132</v>
       </c>
       <c r="Z41" s="1">
-        <f>Y41/X41</f>
+        <f t="shared" si="42"/>
         <v>0.86778580679519945</v>
       </c>
       <c r="AE41" s="1">
-        <f>$AZ$4</f>
+        <f t="shared" si="43"/>
         <v>0.80813377084037297</v>
       </c>
       <c r="AF41" s="1">
@@ -14259,11 +14252,11 @@
         <v>0.67789599744765638</v>
       </c>
       <c r="AG41" s="1">
-        <f>AF41/AE41</f>
+        <f t="shared" si="44"/>
         <v>0.83884131799456518</v>
       </c>
       <c r="AH41" s="1">
-        <f>$BN$4</f>
+        <f t="shared" si="45"/>
         <v>0.77718604816528802</v>
       </c>
       <c r="AI41" s="1">
@@ -14271,7 +14264,7 @@
         <v>0.60079838599950064</v>
       </c>
       <c r="AJ41" s="1">
-        <f>AI41/AH41</f>
+        <f t="shared" si="46"/>
         <v>0.77304319527841792</v>
       </c>
     </row>
@@ -14300,11 +14293,11 @@
       <c r="J42" s="1">
         <v>3109.2930000000001</v>
       </c>
-      <c r="Q42" s="93" t="s">
+      <c r="Q42" s="59" t="s">
         <v>142</v>
       </c>
       <c r="R42" s="1">
-        <f>$J$4</f>
+        <f t="shared" si="37"/>
         <v>0.854229450914883</v>
       </c>
       <c r="S42" s="1">
@@ -14312,11 +14305,11 @@
         <v>0.82902350811129699</v>
       </c>
       <c r="T42" s="1">
-        <f>S42/R42</f>
+        <f t="shared" si="38"/>
         <v>0.97049277243182108</v>
       </c>
       <c r="U42" s="1">
-        <f>$X$4</f>
+        <f t="shared" si="39"/>
         <v>0.82801129151097597</v>
       </c>
       <c r="V42" s="1">
@@ -14324,11 +14317,11 @@
         <v>0.77060614296486341</v>
       </c>
       <c r="W42" s="1">
-        <f>V42/U42</f>
+        <f t="shared" si="40"/>
         <v>0.93067105589664345</v>
       </c>
       <c r="X42" s="1">
-        <f>$AL$4</f>
+        <f t="shared" si="41"/>
         <v>0.80816421943629901</v>
       </c>
       <c r="Y42" s="1">
@@ -14336,11 +14329,11 @@
         <v>0.71176724788023238</v>
       </c>
       <c r="Z42" s="1">
-        <f>Y42/X42</f>
+        <f t="shared" si="42"/>
         <v>0.8807210598567401</v>
       </c>
       <c r="AE42" s="1">
-        <f>$AZ$4</f>
+        <f t="shared" si="43"/>
         <v>0.80813377084037297</v>
       </c>
       <c r="AF42" s="1">
@@ -14348,11 +14341,11 @@
         <v>0.65509737254164901</v>
       </c>
       <c r="AG42" s="1">
-        <f>AF42/AE42</f>
+        <f t="shared" si="44"/>
         <v>0.81062986869168652</v>
       </c>
       <c r="AH42" s="1">
-        <f>$BN$4</f>
+        <f t="shared" si="45"/>
         <v>0.77718604816528802</v>
       </c>
       <c r="AI42" s="1">
@@ -14360,7 +14353,7 @@
         <v>0.57528083138307629</v>
       </c>
       <c r="AJ42" s="1">
-        <f>AI42/AH42</f>
+        <f t="shared" si="46"/>
         <v>0.74020993138148616</v>
       </c>
     </row>
@@ -14393,7 +14386,7 @@
         <v>143</v>
       </c>
       <c r="R43" s="1">
-        <f>$J$4</f>
+        <f t="shared" si="37"/>
         <v>0.854229450914883</v>
       </c>
       <c r="S43" s="1">
@@ -14401,11 +14394,11 @@
         <v>0.79036977414406151</v>
       </c>
       <c r="T43" s="1">
-        <f>S43/R43</f>
+        <f t="shared" si="38"/>
         <v>0.92524294649121785</v>
       </c>
       <c r="U43" s="1">
-        <f>$X$4</f>
+        <f t="shared" si="39"/>
         <v>0.82801129151097597</v>
       </c>
       <c r="V43" s="1">
@@ -14413,11 +14406,11 @@
         <v>0.68326278041566901</v>
       </c>
       <c r="W43" s="1">
-        <f>V43/U43</f>
+        <f t="shared" si="40"/>
         <v>0.82518534157769008</v>
       </c>
       <c r="X43" s="1">
-        <f>$AL$4</f>
+        <f t="shared" si="41"/>
         <v>0.80816421943629901</v>
       </c>
       <c r="Y43" s="1">
@@ -14425,11 +14418,11 @@
         <v>0.57282423944146443</v>
       </c>
       <c r="Z43" s="1">
-        <f>Y43/X43</f>
+        <f t="shared" si="42"/>
         <v>0.70879683319933895</v>
       </c>
       <c r="AE43" s="1">
-        <f>$AZ$4</f>
+        <f t="shared" si="43"/>
         <v>0.80813377084037297</v>
       </c>
       <c r="AF43" s="1">
@@ -14437,11 +14430,11 @@
         <v>0.65003224521428793</v>
       </c>
       <c r="AG43" s="1">
-        <f>AF43/AE43</f>
+        <f t="shared" si="44"/>
         <v>0.80436218441697305</v>
       </c>
       <c r="AH43" s="1">
-        <f>$BN$4</f>
+        <f t="shared" si="45"/>
         <v>0.77718604816528802</v>
       </c>
       <c r="AI43" s="1">
@@ -14449,7 +14442,7 @@
         <v>0.57408082559471674</v>
       </c>
       <c r="AJ43" s="1">
-        <f>AI43/AH43</f>
+        <f t="shared" si="46"/>
         <v>0.73866589209875277</v>
       </c>
     </row>
@@ -14482,7 +14475,7 @@
         <v>144</v>
       </c>
       <c r="R44" s="1">
-        <f>$J$4</f>
+        <f t="shared" si="37"/>
         <v>0.854229450914883</v>
       </c>
       <c r="S44" s="1">
@@ -14490,11 +14483,11 @@
         <v>0.75560587531784407</v>
       </c>
       <c r="T44" s="1">
-        <f>S44/R44</f>
+        <f t="shared" si="38"/>
         <v>0.88454673917948778</v>
       </c>
       <c r="U44" s="1">
-        <f>$X$4</f>
+        <f t="shared" si="39"/>
         <v>0.82801129151097597</v>
       </c>
       <c r="V44" s="1">
@@ -14502,11 +14495,11 @@
         <v>0.65824418577235899</v>
       </c>
       <c r="W44" s="1">
-        <f>V44/U44</f>
+        <f t="shared" si="40"/>
         <v>0.79497005961256684</v>
       </c>
       <c r="X44" s="1">
-        <f>$AL$4</f>
+        <f t="shared" si="41"/>
         <v>0.80816421943629901</v>
       </c>
       <c r="Y44" s="1">
@@ -14514,11 +14507,11 @@
         <v>0.55210426365353305</v>
       </c>
       <c r="Z44" s="1">
-        <f>Y44/X44</f>
+        <f t="shared" si="42"/>
         <v>0.68315850958933833</v>
       </c>
       <c r="AE44" s="1">
-        <f>$AZ$4</f>
+        <f t="shared" si="43"/>
         <v>0.80813377084037297</v>
       </c>
       <c r="AF44" s="1">
@@ -14526,11 +14519,11 @@
         <v>0.56038890758132831</v>
       </c>
       <c r="AG44" s="1">
-        <f>AF44/AE44</f>
+        <f t="shared" si="44"/>
         <v>0.69343582436677975</v>
       </c>
       <c r="AH44" s="1">
-        <f>$BN$4</f>
+        <f t="shared" si="45"/>
         <v>0.77718604816528802</v>
       </c>
       <c r="AI44" s="1">
@@ -14538,7 +14531,7 @@
         <v>0.4774360235468007</v>
       </c>
       <c r="AJ44" s="1">
-        <f>AI44/AH44</f>
+        <f t="shared" si="46"/>
         <v>0.61431368289985311</v>
       </c>
     </row>
@@ -14551,31 +14544,31 @@
         <v>44100</v>
       </c>
       <c r="D45" s="1">
-        <f t="shared" ref="D45:J45" si="37">AVERAGE(D42:D44)</f>
+        <f t="shared" ref="D45:J45" si="47">AVERAGE(D42:D44)</f>
         <v>301.32499999999999</v>
       </c>
       <c r="E45" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="47"/>
         <v>2</v>
       </c>
       <c r="F45" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="47"/>
         <v>4.9989999999999997</v>
       </c>
       <c r="G45" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="47"/>
         <v>4.7903333333333329</v>
       </c>
-      <c r="H45" s="4">
-        <f t="shared" si="37"/>
+      <c r="H45" s="1">
+        <f t="shared" si="47"/>
         <v>3.2466666666666665E-2</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="47"/>
         <v>3517.72</v>
       </c>
       <c r="J45" s="1">
-        <f t="shared" si="37"/>
+        <f t="shared" si="47"/>
         <v>3113.1120000000005</v>
       </c>
       <c r="Q45" s="1" t="s">
@@ -14590,7 +14583,7 @@
         <v>0.82986196958001868</v>
       </c>
       <c r="T45" s="1">
-        <f>S45/R45</f>
+        <f t="shared" si="38"/>
         <v>0.98597027264358905</v>
       </c>
       <c r="U45" s="1">
@@ -14602,7 +14595,7 @@
         <v>0.78704952670881534</v>
       </c>
       <c r="W45" s="1">
-        <f>V45/U45</f>
+        <f t="shared" si="40"/>
         <v>0.96676566671312847</v>
       </c>
       <c r="X45" s="1">
@@ -14614,7 +14607,7 @@
         <v>0.73125729917705173</v>
       </c>
       <c r="Z45" s="1">
-        <f>Y45/X45</f>
+        <f t="shared" si="42"/>
         <v>0.91877548901240513</v>
       </c>
       <c r="AE45" s="1">
@@ -14626,7 +14619,7 @@
         <v>0.65489751649281636</v>
       </c>
       <c r="AG45" s="1">
-        <f>AF45/AE45</f>
+        <f t="shared" si="44"/>
         <v>0.81654152441091243</v>
       </c>
       <c r="AH45" s="1">
@@ -14638,19 +14631,38 @@
         <v>0.57178110417225037</v>
       </c>
       <c r="AJ45" s="1">
-        <f>AI45/AH45</f>
+        <f t="shared" si="46"/>
         <v>0.73953557407660753</v>
+      </c>
+    </row>
+    <row r="49" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="B49" s="47" t="s">
+        <v>147</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="50" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="C50" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E50" s="1">
+        <v>38526</v>
+      </c>
+    </row>
+    <row r="51" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E51" s="1">
+        <v>39634</v>
+      </c>
+    </row>
+    <row r="52" spans="2:5" x14ac:dyDescent="0.45">
+      <c r="E52" s="1">
+        <v>38352</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="R36:Z36"/>
-    <mergeCell ref="AE37:AG37"/>
-    <mergeCell ref="AH37:AJ37"/>
-    <mergeCell ref="AE36:AJ36"/>
-    <mergeCell ref="U37:W37"/>
-    <mergeCell ref="X37:Z37"/>
-    <mergeCell ref="R37:T37"/>
     <mergeCell ref="AR1:BE1"/>
     <mergeCell ref="BF1:BS1"/>
     <mergeCell ref="AD1:AQ1"/>
@@ -14664,6 +14676,13 @@
     <mergeCell ref="A12:A14"/>
     <mergeCell ref="A15:A18"/>
     <mergeCell ref="A19:A21"/>
+    <mergeCell ref="R36:Z36"/>
+    <mergeCell ref="AE37:AG37"/>
+    <mergeCell ref="AH37:AJ37"/>
+    <mergeCell ref="AE36:AJ36"/>
+    <mergeCell ref="U37:W37"/>
+    <mergeCell ref="X37:Z37"/>
+    <mergeCell ref="R37:T37"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="T39:T45">

</xml_diff>